<commit_message>
apply changes to excel sheets
</commit_message>
<xml_diff>
--- a/pendulum/random_full_grav/random_full_grav.xlsx
+++ b/pendulum/random_full_grav/random_full_grav.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/random_full_grav/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191E6474-7BE2-904A-A56A-817248CC8439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6264A7-145A-5B4A-8F8C-73AD94ACEE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="9.81" sheetId="2" r:id="rId2"/>
+    <sheet name="13" sheetId="2" r:id="rId2"/>
+    <sheet name="15" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,9 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>empty</t>
+  </si>
+  <si>
+    <t>Ind</t>
   </si>
   <si>
     <t>conditional(add(add(y, y), y), add(add(add(vel, add(x, add(conditional(y, conditional(y, conditional(conditional(conditional(conditional(x, add(vel, y)), x), conditional(add(vel, vel), add(add(add(y, y), add(add(x, x), add(y, x))), vel))), vel))), conditional(x, x)))), x), add(add(x, y), y)))</t>
@@ -63,10 +67,37 @@
     <t>conditional(add(y, y), add(add(add(x, x), add(add(x, x), conditional(x, x))), add(add(vel, vel), add(add(add(x, x), add(add(x, add(conditional(x, add(add(add(add(add(add(vel, y), add(x, x)), add(conditional(vel, x), add(x, vel))), x), add(vel, y)), conditional(x, add(add(vel, add(conditional(x, vel), x)), add(vel, conditional(conditional(conditional(y, x), conditional(y, x)), conditional(x, conditional(add(vel, y), add(x, x))))))))), conditional(y, vel))), x)), y))))</t>
   </si>
   <si>
-    <t>Ind</t>
+    <t>Fit</t>
   </si>
   <si>
-    <t>Fit</t>
+    <t>conditional(add(y, add(conditional(y, y), y)), add(add(add(x, add(x, add(conditional(add(x, conditional(y, y)), conditional(conditional(x, add(x, add(y, add(y, add(conditional(conditional(vel, vel), conditional(y, x)), conditional(vel, x)))))), add(add(vel, vel), conditional(conditional(y, x), y)))), vel))), add(add(add(x, add(conditional(conditional(x, x), add(add(add(x, x), vel), conditional(conditional(conditional(x, vel), add(conditional(conditional(y, y), add(x, y)), add(y, add(conditional(add(x, y), add(x, x)), conditional(conditional(vel, y), add(vel, vel)))))), conditional(conditional(vel, y), conditional(vel, vel))))), add(add(add(vel, x), conditional(vel, add(conditional(conditional(conditional(vel, vel), add(vel, y)), y), conditional(y, x)))), vel))), conditional(add(conditional(x, vel), x), conditional(x, conditional(add(y, vel), add(y, vel))))), add(y, x))), add(add(x, y), x)))</t>
+  </si>
+  <si>
+    <t>conditional(add(add(y, conditional(x, conditional(conditional(conditional(x, vel), add(add(y, x), vel)), add(y, x)))), y), add(add(x, add(add(vel, y), conditional(x, x))), add(add(conditional(y, conditional(y, conditional(conditional(conditional(add(x, add(vel, vel)), add(x, add(conditional(x, vel), conditional(x, vel)))), x), add(add(x, add(add(vel, y), add(y, conditional(x, conditional(conditional(conditional(x, vel), add(add(add(vel, x), conditional(y, y)), vel)), add(y, x)))))), add(add(conditional(y, conditional(y, add(add(y, add(conditional(x, y), conditional(y, x))), conditional(x, vel)))), add(x, conditional(x, vel))), x))))), x), x)))</t>
+  </si>
+  <si>
+    <t>conditional(add(y, conditional(add(y, y), add(y, y))), add(add(add(conditional(x, y), conditional(x, x)), vel), add(x, add(conditional(conditional(x, vel), add(conditional(add(add(vel, conditional(y, x)), add(y, y)), x), vel)), add(x, add(add(add(y, x), y), add(x, conditional(y, x))))))))</t>
+  </si>
+  <si>
+    <t>conditional(add(add(add(y, y), y), y), add(add(x, add(conditional(conditional(x, add(conditional(add(conditional(x, y), y), x), add(conditional(x, vel), x))), conditional(conditional(add(add(y, y), conditional(y, vel)), conditional(add(add(add(conditional(y, y), x), conditional(y, x)), vel), conditional(add(conditional(vel, vel), add(vel, add(y, vel))), vel))), conditional(conditional(conditional(conditional(x, y), x), conditional(y, y)), conditional(vel, x)))), add(x, x))), add(y, add(add(add(x, y), vel), add(y, y)))))</t>
+  </si>
+  <si>
+    <t>conditional(add(add(y, y), y), add(add(x, add(x, x)), add(add(add(vel, add(add(conditional(conditional(add(add(vel, y), conditional(vel, y)), conditional(add(x, y), y)), conditional(add(add(y, y), conditional(x, x)), add(x, add(x, add(x, x))))), add(y, x)), add(add(vel, x), add(x, x)))), add(add(conditional(add(vel, vel), add(add(add(y, vel), add(y, vel)), add(x, add(conditional(conditional(y, x), x), conditional(y, y))))), add(y, x)), add(add(vel, x), add(x, x)))), vel)))</t>
+  </si>
+  <si>
+    <t>conditional(add(y, add(y, add(y, y))), add(add(add(add(add(x, add(x, x)), add(vel, x)), y), conditional(x, x)), add(add(add(add(add(add(add(conditional(vel, y), conditional(add(x, y), conditional(y, add(y, x)))), add(x, x)), conditional(add(vel, x), add(vel, vel))), add(x, add(x, add(conditional(vel, vel), add(add(vel, add(y, x)), x))))), y), add(add(y, x), x)), conditional(x, y))))</t>
+  </si>
+  <si>
+    <t>conditional(add(y, add(add(y, x), add(conditional(y, y), y))), add(add(add(conditional(conditional(y, vel), conditional(add(add(y, y), conditional(y, add(add(add(x, x), add(y, y)), x))), add(vel, vel))), add(x, add(add(add(add(vel, y), add(add(y, vel), x)), x), add(x, add(x, x))))), x), add(x, add(add(y, add(add(add(x, add(x, x)), add(x, add(add(add(conditional(vel, vel), x), add(x, y)), conditional(conditional(x, add(conditional(x, x), vel)), conditional(add(conditional(vel, vel), add(y, add(conditional(add(y, y), add(vel, vel)), add(y, y)))), x))))), x)), x))))</t>
+  </si>
+  <si>
+    <t>conditional(add(add(y, y), add(y, y)), add(add(add(add(add(add(y, add(add(vel, y), add(x, x))), add(conditional(y, y), add(y, x))), add(add(x, x), conditional(conditional(x, y), add(x, conditional(add(y, y), add(x, y)))))), conditional(vel, vel)), x), x))</t>
+  </si>
+  <si>
+    <t>add(conditional(x, add(x, add(add(y, add(add(conditional(add(x, add(add(add(add(x, x), add(add(add(x, x), x), add(add(x, x), x))), add(x, vel)), x)), x), conditional(conditional(conditional(x, vel), y), add(y, y))), conditional(add(vel, vel), conditional(y, x)))), conditional(add(add(conditional(vel, x), vel), conditional(conditional(vel, x), conditional(vel, y))), add(y, vel))))), conditional(add(y, y), add(vel, add(add(add(add(add(add(add(x, x), x), add(y, x)), y), add(conditional(x, add(vel, x)), add(x, x))), add(conditional(x, x), vel)), x))))</t>
+  </si>
+  <si>
+    <t>conditional(add(add(y, y), add(y, x)), add(add(add(y, x), add(add(x, y), add(x, x))), add(add(y, add(vel, x)), conditional(conditional(x, add(conditional(add(conditional(add(add(x, conditional(add(x, x), add(add(vel, x), conditional(y, vel)))), add(conditional(conditional(vel, add(add(y, x), conditional(x, vel))), add(conditional(conditional(vel, y), vel), conditional(x, vel))), vel)), vel), add(conditional(vel, y), add(vel, x))), conditional(conditional(conditional(conditional(x, add(conditional(y, x), add(y, vel))), conditional(add(x, x), conditional(y, y))), add(conditional(add(vel, vel), x), conditional(x, vel))), y)), add(conditional(conditional(x, y), conditional(x, y)), conditional(conditional(x, add(conditional(vel, conditional(conditional(conditional(x, x), add(add(vel, y), add(add(add(y, y), add(vel, x)), add(y, vel)))), add(x, y))), add(conditional(add(conditional(conditional(y, add(vel, x)), conditional(x, y)), add(add(vel, add(add(x, y), add(y, vel))), conditional(add(x, y), x))), conditional(add(vel, y), x)), conditional(add(x, vel), add(vel, x))))), add(conditional(add(y, vel), conditional(conditional(vel, conditional(conditional(vel, conditional(conditional(x, vel), vel)), add(conditional(conditional(add(y, x), x), y), conditional(x, x)))), add(conditional(y, y), conditional(y, x)))), add(x, y)))))), add(conditional(add(y, vel), conditional(conditional(vel, conditional(add(y, add(y, add(vel, x))), add(conditional(add(add(conditional(x, y), add(x, vel)), add(conditional(conditional(vel, conditional(conditional(vel, x), add(vel, vel))), add(conditional(add(x, vel), vel), conditional(x, vel))), vel)), vel), add(conditional(vel, x), add(conditional(x, y), x))))), y)), conditional(conditional(x, conditional(conditional(x, vel), y)), add(add(x, y), conditional(y, conditional(x, x)))))))))</t>
   </si>
 </sst>
 </file>
@@ -136,6 +167,352 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>None</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'13'!$B$11:$Q$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'9.81'!#REF!</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-194.38749999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-191.83875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-182.14875000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-180.8725</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-189.86875000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-196.5675</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-211.73750000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-195.185</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-215.4725</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-216.58875</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-228.09875</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-256.51375000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-944.80124999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1483.8687500000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1644.6925000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1790.8275000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'9.81'!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Fit</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1887-E741-82C3-8E172A801702}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1074713648"/>
+        <c:axId val="1531991088"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1074713648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1531991088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1531991088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1074713648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -176,7 +553,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'9.81'!$A$11</c:f>
+              <c:f>'15'!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -199,7 +576,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'9.81'!$B$10:$Q$10</c:f>
+              <c:f>'15'!$B$13:$Q$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -256,57 +633,57 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'9.81'!$B$11:$Q$11</c:f>
+              <c:f>'15'!$B$14:$Q$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>-194.38749999999999</c:v>
+                  <c:v>-134.446</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-191.83875</c:v>
+                  <c:v>-126.43200000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-182.14875000000001</c:v>
+                  <c:v>-137.16399999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-180.8725</c:v>
+                  <c:v>-143.74699999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-189.86875000000001</c:v>
+                  <c:v>-162.54400000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-196.5675</c:v>
+                  <c:v>-176.85300000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-211.73750000000001</c:v>
+                  <c:v>-170.24900000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-195.185</c:v>
+                  <c:v>-186.14800000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-215.47250000000003</c:v>
+                  <c:v>-194.95500000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-216.58875</c:v>
+                  <c:v>-205.99299999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-228.09875</c:v>
+                  <c:v>-221.80700000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-256.51375000000002</c:v>
+                  <c:v>-228.94399999999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-944.80124999999998</c:v>
+                  <c:v>-316.56899999999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-1483.8687499999996</c:v>
+                  <c:v>-784.322</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1644.6925000000001</c:v>
+                  <c:v>-1543.931</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1790.8275000000003</c:v>
+                  <c:v>-1681.5169999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -314,7 +691,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C68A-B041-B1E0-BD931F2A08B2}"/>
+              <c16:uniqueId val="{00000000-7878-9D48-AC6F-BF602411C75A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -327,11 +704,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1074713648"/>
-        <c:axId val="1531991088"/>
+        <c:axId val="1208166048"/>
+        <c:axId val="1208154272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1074713648"/>
+        <c:axId val="1208166048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -374,7 +751,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1531991088"/>
+        <c:crossAx val="1208154272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -382,9 +759,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1531991088"/>
+        <c:axId val="1208154272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="-2000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -433,7 +811,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1074713648"/>
+        <c:crossAx val="1208166048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1065,7 +1443,48 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0296C5E-9883-9B72-9DEE-F130F5577105}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D636F47-F0BE-B307-8B17-8D3E18D5A6C9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1386,7 +1805,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1403,17 +1822,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -1469,52 +1888,52 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-144.79</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>-165.52</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>-141.1</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>-177.26</v>
+        <v>4</v>
       </c>
       <c r="F2">
-        <v>-158.30000000000001</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>-171.49</v>
+        <v>6</v>
       </c>
       <c r="H2">
-        <v>-187.61</v>
+        <v>7</v>
       </c>
       <c r="I2">
-        <v>-183.55</v>
+        <v>8</v>
       </c>
       <c r="J2">
-        <v>-202.67</v>
+        <v>9.81</v>
       </c>
       <c r="K2">
-        <v>-244.01</v>
+        <v>11</v>
       </c>
       <c r="L2">
-        <v>-217.68</v>
+        <v>12</v>
       </c>
       <c r="M2">
-        <v>-232.62</v>
+        <v>13</v>
       </c>
       <c r="N2">
-        <v>-729.37</v>
+        <v>14</v>
       </c>
       <c r="O2">
-        <v>-1419.86</v>
+        <v>15</v>
       </c>
       <c r="P2">
-        <v>-1648.98</v>
+        <v>16</v>
       </c>
       <c r="Q2">
-        <v>-1749.75</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -1522,52 +1941,52 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-174.77</v>
+        <v>-144.79</v>
       </c>
       <c r="C3">
-        <v>-145.4</v>
+        <v>-165.52</v>
       </c>
       <c r="D3">
-        <v>-182.09</v>
+        <v>-141.1</v>
       </c>
       <c r="E3">
-        <v>-125.31</v>
+        <v>-177.26</v>
       </c>
       <c r="F3">
-        <v>-148.87</v>
+        <v>-158.30000000000001</v>
       </c>
       <c r="G3">
-        <v>-165.02</v>
+        <v>-171.49</v>
       </c>
       <c r="H3">
-        <v>-160.97</v>
+        <v>-187.61</v>
       </c>
       <c r="I3">
-        <v>-167.19</v>
+        <v>-183.55</v>
       </c>
       <c r="J3">
-        <v>-206.26</v>
+        <v>-202.67</v>
       </c>
       <c r="K3">
-        <v>-185.81</v>
+        <v>-244.01</v>
       </c>
       <c r="L3">
-        <v>-213.59</v>
+        <v>-217.68</v>
       </c>
       <c r="M3">
-        <v>-239.81</v>
+        <v>-232.62</v>
       </c>
       <c r="N3">
-        <v>-1115.77</v>
+        <v>-729.37</v>
       </c>
       <c r="O3">
-        <v>-1481.79</v>
+        <v>-1419.86</v>
       </c>
       <c r="P3">
-        <v>-1594.41</v>
+        <v>-1648.98</v>
       </c>
       <c r="Q3">
-        <v>-1762.18</v>
+        <v>-1749.75</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1575,52 +1994,52 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-138.22</v>
+        <v>-174.77</v>
       </c>
       <c r="C4">
-        <v>-130.41999999999999</v>
+        <v>-145.4</v>
       </c>
       <c r="D4">
-        <v>-173.22</v>
+        <v>-182.09</v>
       </c>
       <c r="E4">
-        <v>-170.63</v>
+        <v>-125.31</v>
       </c>
       <c r="F4">
-        <v>-177.82</v>
+        <v>-148.87</v>
       </c>
       <c r="G4">
-        <v>-184.06</v>
+        <v>-165.02</v>
       </c>
       <c r="H4">
-        <v>-197.36</v>
+        <v>-160.97</v>
       </c>
       <c r="I4">
-        <v>-193.96</v>
+        <v>-167.19</v>
       </c>
       <c r="J4">
-        <v>-212.77</v>
+        <v>-206.26</v>
       </c>
       <c r="K4">
-        <v>-255.75</v>
+        <v>-185.81</v>
       </c>
       <c r="L4">
-        <v>-294.14</v>
+        <v>-213.59</v>
       </c>
       <c r="M4">
-        <v>-324.68</v>
+        <v>-239.81</v>
       </c>
       <c r="N4">
-        <v>-1391.5</v>
+        <v>-1115.77</v>
       </c>
       <c r="O4">
-        <v>-1616.33</v>
+        <v>-1481.79</v>
       </c>
       <c r="P4">
-        <v>-1683.17</v>
+        <v>-1594.41</v>
       </c>
       <c r="Q4">
-        <v>-1856.04</v>
+        <v>-1762.18</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -1628,52 +2047,52 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-211.15</v>
+        <v>-138.22</v>
       </c>
       <c r="C5">
-        <v>-228.47</v>
+        <v>-130.41999999999999</v>
       </c>
       <c r="D5">
-        <v>-235.07</v>
+        <v>-173.22</v>
       </c>
       <c r="E5">
-        <v>-206.46</v>
+        <v>-170.63</v>
       </c>
       <c r="F5">
-        <v>-255.92</v>
+        <v>-177.82</v>
       </c>
       <c r="G5">
-        <v>-216.91</v>
+        <v>-184.06</v>
       </c>
       <c r="H5">
-        <v>-261.95999999999998</v>
+        <v>-197.36</v>
       </c>
       <c r="I5">
-        <v>-213.46</v>
+        <v>-193.96</v>
       </c>
       <c r="J5">
-        <v>-195.3</v>
+        <v>-212.77</v>
       </c>
       <c r="K5">
-        <v>-181.47</v>
+        <v>-255.75</v>
       </c>
       <c r="L5">
-        <v>-186.06</v>
+        <v>-294.14</v>
       </c>
       <c r="M5">
-        <v>-209.38</v>
+        <v>-324.68</v>
       </c>
       <c r="N5">
-        <v>-258.75</v>
+        <v>-1391.5</v>
       </c>
       <c r="O5">
-        <v>-1340.06</v>
+        <v>-1616.33</v>
       </c>
       <c r="P5">
-        <v>-1636.01</v>
+        <v>-1683.17</v>
       </c>
       <c r="Q5">
-        <v>-1804.48</v>
+        <v>-1856.04</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -1681,52 +2100,52 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-187.85</v>
+        <v>-211.15</v>
       </c>
       <c r="C6">
-        <v>-173.05</v>
+        <v>-228.47</v>
       </c>
       <c r="D6">
-        <v>-154.04</v>
+        <v>-235.07</v>
       </c>
       <c r="E6">
-        <v>-161.04</v>
+        <v>-206.46</v>
       </c>
       <c r="F6">
-        <v>-174.16</v>
+        <v>-255.92</v>
       </c>
       <c r="G6">
-        <v>-177.7</v>
+        <v>-216.91</v>
       </c>
       <c r="H6">
-        <v>-195.09</v>
+        <v>-261.95999999999998</v>
       </c>
       <c r="I6">
-        <v>-220.15</v>
+        <v>-213.46</v>
       </c>
       <c r="J6">
-        <v>-251</v>
+        <v>-195.3</v>
       </c>
       <c r="K6">
-        <v>-240.41</v>
+        <v>-181.47</v>
       </c>
       <c r="L6">
-        <v>-253.25</v>
+        <v>-186.06</v>
       </c>
       <c r="M6">
-        <v>-307.17</v>
+        <v>-209.38</v>
       </c>
       <c r="N6">
-        <v>-1341.49</v>
+        <v>-258.75</v>
       </c>
       <c r="O6">
-        <v>-1632.21</v>
+        <v>-1340.06</v>
       </c>
       <c r="P6">
-        <v>-1739.47</v>
+        <v>-1636.01</v>
       </c>
       <c r="Q6">
-        <v>-1840.85</v>
+        <v>-1804.48</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -1734,52 +2153,52 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-297.8</v>
+        <v>-187.85</v>
       </c>
       <c r="C7">
-        <v>-316.06</v>
+        <v>-173.05</v>
       </c>
       <c r="D7">
-        <v>-236.99</v>
+        <v>-154.04</v>
       </c>
       <c r="E7">
-        <v>-203.92</v>
+        <v>-161.04</v>
       </c>
       <c r="F7">
-        <v>-161.91</v>
+        <v>-174.16</v>
       </c>
       <c r="G7">
-        <v>-177.67</v>
+        <v>-177.7</v>
       </c>
       <c r="H7">
-        <v>-172.71</v>
+        <v>-195.09</v>
       </c>
       <c r="I7">
-        <v>-166.92</v>
+        <v>-220.15</v>
       </c>
       <c r="J7">
-        <v>-190.67</v>
+        <v>-251</v>
       </c>
       <c r="K7">
-        <v>-184.74</v>
+        <v>-240.41</v>
       </c>
       <c r="L7">
-        <v>-205.05</v>
+        <v>-253.25</v>
       </c>
       <c r="M7">
-        <v>-226.69</v>
+        <v>-307.17</v>
       </c>
       <c r="N7">
-        <v>-300.07</v>
+        <v>-1341.49</v>
       </c>
       <c r="O7">
-        <v>-1394.58</v>
+        <v>-1632.21</v>
       </c>
       <c r="P7">
-        <v>-1476.16</v>
+        <v>-1739.47</v>
       </c>
       <c r="Q7">
-        <v>-1743.69</v>
+        <v>-1840.85</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -1787,52 +2206,52 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-182.13</v>
+        <v>-297.8</v>
       </c>
       <c r="C8">
-        <v>-197.23</v>
+        <v>-316.06</v>
       </c>
       <c r="D8">
-        <v>-171.95</v>
+        <v>-236.99</v>
       </c>
       <c r="E8">
-        <v>-213.96</v>
+        <v>-203.92</v>
       </c>
       <c r="F8">
-        <v>-274.73</v>
+        <v>-161.91</v>
       </c>
       <c r="G8">
-        <v>-281.07</v>
+        <v>-177.67</v>
       </c>
       <c r="H8">
-        <v>-274.41000000000003</v>
+        <v>-172.71</v>
       </c>
       <c r="I8">
-        <v>-227.74</v>
+        <v>-166.92</v>
       </c>
       <c r="J8">
-        <v>-236.7</v>
+        <v>-190.67</v>
       </c>
       <c r="K8">
-        <v>-207.46</v>
+        <v>-184.74</v>
       </c>
       <c r="L8">
-        <v>-239.05</v>
+        <v>-205.05</v>
       </c>
       <c r="M8">
-        <v>-281.19</v>
+        <v>-226.69</v>
       </c>
       <c r="N8">
-        <v>-1390.66</v>
+        <v>-300.07</v>
       </c>
       <c r="O8">
-        <v>-1508.14</v>
+        <v>-1394.58</v>
       </c>
       <c r="P8">
-        <v>-1695.53</v>
+        <v>-1476.16</v>
       </c>
       <c r="Q8">
-        <v>-1765.78</v>
+        <v>-1743.69</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -1840,171 +2259,992 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-218.39</v>
+        <v>-182.13</v>
       </c>
       <c r="C9">
-        <v>-178.56</v>
+        <v>-197.23</v>
       </c>
       <c r="D9">
-        <v>-162.72999999999999</v>
+        <v>-171.95</v>
       </c>
       <c r="E9">
-        <v>-188.4</v>
+        <v>-213.96</v>
       </c>
       <c r="F9">
-        <v>-167.24</v>
+        <v>-274.73</v>
       </c>
       <c r="G9">
-        <v>-198.62</v>
+        <v>-281.07</v>
       </c>
       <c r="H9">
-        <v>-243.79</v>
+        <v>-274.41000000000003</v>
       </c>
       <c r="I9">
-        <v>-188.51</v>
+        <v>-227.74</v>
       </c>
       <c r="J9">
-        <v>-228.41</v>
+        <v>-236.7</v>
       </c>
       <c r="K9">
-        <v>-233.06</v>
+        <v>-207.46</v>
       </c>
       <c r="L9">
-        <v>-215.97</v>
+        <v>-239.05</v>
       </c>
       <c r="M9">
-        <v>-230.57</v>
+        <v>-281.19</v>
       </c>
       <c r="N9">
-        <v>-1030.8</v>
+        <v>-1390.66</v>
       </c>
       <c r="O9">
-        <v>-1477.98</v>
+        <v>-1508.14</v>
       </c>
       <c r="P9">
-        <v>-1683.81</v>
+        <v>-1695.53</v>
       </c>
       <c r="Q9">
-        <v>-1803.85</v>
+        <v>-1765.78</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
       <c r="B10">
+        <v>-218.39</v>
+      </c>
+      <c r="C10">
+        <v>-178.56</v>
+      </c>
+      <c r="D10">
+        <v>-162.72999999999999</v>
+      </c>
+      <c r="E10">
+        <v>-188.4</v>
+      </c>
+      <c r="F10">
+        <v>-167.24</v>
+      </c>
+      <c r="G10">
+        <v>-198.62</v>
+      </c>
+      <c r="H10">
+        <v>-243.79</v>
+      </c>
+      <c r="I10">
+        <v>-188.51</v>
+      </c>
+      <c r="J10">
+        <v>-228.41</v>
+      </c>
+      <c r="K10">
+        <v>-233.06</v>
+      </c>
+      <c r="L10">
+        <v>-215.97</v>
+      </c>
+      <c r="M10">
+        <v>-230.57</v>
+      </c>
+      <c r="N10">
+        <v>-1030.8</v>
+      </c>
+      <c r="O10">
+        <v>-1477.98</v>
+      </c>
+      <c r="P10">
+        <v>-1683.81</v>
+      </c>
+      <c r="Q10">
+        <v>-1803.85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B11">
         <v>1</v>
       </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <v>8</v>
+      </c>
+      <c r="J11">
+        <v>9.81</v>
+      </c>
+      <c r="K11">
+        <v>11</v>
+      </c>
+      <c r="L11">
+        <v>12</v>
+      </c>
+      <c r="M11">
+        <v>13</v>
+      </c>
+      <c r="N11">
+        <v>14</v>
+      </c>
+      <c r="O11">
+        <v>15</v>
+      </c>
+      <c r="P11">
+        <v>16</v>
+      </c>
+      <c r="Q11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <v>7</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <v>9.81</v>
+      </c>
+      <c r="K13">
+        <v>11</v>
+      </c>
+      <c r="L13">
+        <v>12</v>
+      </c>
+      <c r="M13">
+        <v>13</v>
+      </c>
+      <c r="N13">
+        <v>14</v>
+      </c>
+      <c r="O13">
+        <v>15</v>
+      </c>
+      <c r="P13">
+        <v>16</v>
+      </c>
+      <c r="Q13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f>AVERAGE(B2:B11)</f>
+        <v>-155.31</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:Q14" si="0">AVERAGE(C2:C11)</f>
+        <v>-153.071</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-145.119</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>-143.898</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>-150.89500000000001</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>-156.054</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>-167.99</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>-154.548</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>-170.41600000000003</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>-171.071</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>-180.07900000000001</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>-202.61100000000002</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>-753.04099999999994</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>-1184.0949999999998</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>-1312.5540000000001</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>-1429.2620000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Q14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9.81</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>12</v>
+      </c>
+      <c r="M1">
+        <v>13</v>
+      </c>
+      <c r="N1">
+        <v>14</v>
+      </c>
+      <c r="O1">
+        <v>15</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="Q1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>-155.97</v>
+      </c>
+      <c r="C2">
+        <v>-123.65</v>
+      </c>
+      <c r="D2">
+        <v>-173.25</v>
+      </c>
+      <c r="E2">
+        <v>-144.44999999999999</v>
+      </c>
+      <c r="F2">
+        <v>-156.19</v>
+      </c>
+      <c r="G2">
+        <v>-178.47</v>
+      </c>
+      <c r="H2">
+        <v>-187.63</v>
+      </c>
+      <c r="I2">
+        <v>-168.83</v>
+      </c>
+      <c r="J2">
+        <v>-177</v>
+      </c>
+      <c r="K2">
+        <v>-196.58</v>
+      </c>
+      <c r="L2">
+        <v>-199.08</v>
+      </c>
+      <c r="M2">
+        <v>-236.5</v>
+      </c>
+      <c r="N2">
+        <v>-258.51</v>
+      </c>
+      <c r="O2">
+        <v>-1092.1199999999999</v>
+      </c>
+      <c r="P2">
+        <v>-1600.51</v>
+      </c>
+      <c r="Q2">
+        <v>-1712.94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>-85.38</v>
+      </c>
+      <c r="C3">
+        <v>-95.44</v>
+      </c>
+      <c r="D3">
+        <v>-95.54</v>
+      </c>
+      <c r="E3">
+        <v>-107.69</v>
+      </c>
+      <c r="F3">
+        <v>-114.55</v>
+      </c>
+      <c r="G3">
+        <v>-138.68</v>
+      </c>
+      <c r="H3">
+        <v>-145.88</v>
+      </c>
+      <c r="I3">
+        <v>-176.41</v>
+      </c>
+      <c r="J3">
+        <v>-223.04</v>
+      </c>
+      <c r="K3">
+        <v>-268.73</v>
+      </c>
+      <c r="L3">
+        <v>-391.07</v>
+      </c>
+      <c r="M3">
+        <v>-344.78</v>
+      </c>
+      <c r="N3">
+        <v>-416.86</v>
+      </c>
+      <c r="O3">
+        <v>-575.91</v>
+      </c>
+      <c r="P3">
+        <v>-1556.9</v>
+      </c>
+      <c r="Q3">
+        <v>-1727.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>-134.38</v>
+      </c>
+      <c r="C4">
+        <v>-153.08000000000001</v>
+      </c>
+      <c r="D4">
+        <v>-126.96</v>
+      </c>
+      <c r="E4">
+        <v>-154.02000000000001</v>
+      </c>
+      <c r="F4">
+        <v>-191.94</v>
+      </c>
+      <c r="G4">
+        <v>-182.74</v>
+      </c>
+      <c r="H4">
+        <v>-181.74</v>
+      </c>
+      <c r="I4">
+        <v>-220.15</v>
+      </c>
+      <c r="J4">
+        <v>-195.63</v>
+      </c>
+      <c r="K4">
+        <v>-197.6</v>
+      </c>
+      <c r="L4">
+        <v>-230.94</v>
+      </c>
+      <c r="M4">
+        <v>-215.05</v>
+      </c>
+      <c r="N4">
+        <v>-241.29</v>
+      </c>
+      <c r="O4">
+        <v>-1264.43</v>
+      </c>
+      <c r="P4">
+        <v>-1565.99</v>
+      </c>
+      <c r="Q4">
+        <v>-1686.79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>-126.81</v>
+      </c>
+      <c r="C5">
+        <v>-121.9</v>
+      </c>
+      <c r="D5">
+        <v>-132.53</v>
+      </c>
+      <c r="E5">
+        <v>-133.19999999999999</v>
+      </c>
+      <c r="F5">
+        <v>-152.81</v>
+      </c>
+      <c r="G5">
+        <v>-167.91</v>
+      </c>
+      <c r="H5">
+        <v>-164.63</v>
+      </c>
+      <c r="I5">
+        <v>-202.47</v>
+      </c>
+      <c r="J5">
+        <v>-215.61</v>
+      </c>
+      <c r="K5">
+        <v>-193.56</v>
+      </c>
+      <c r="L5">
+        <v>-193.86</v>
+      </c>
+      <c r="M5">
+        <v>-210.05</v>
+      </c>
+      <c r="N5">
+        <v>-254.75</v>
+      </c>
+      <c r="O5">
+        <v>-801.34</v>
+      </c>
+      <c r="P5">
+        <v>-1570.81</v>
+      </c>
+      <c r="Q5">
+        <v>-1647.61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>-116.93</v>
+      </c>
+      <c r="C6">
+        <v>-131.38999999999999</v>
+      </c>
+      <c r="D6">
+        <v>-124.91</v>
+      </c>
+      <c r="E6">
+        <v>-162.25</v>
+      </c>
+      <c r="F6">
+        <v>-175.94</v>
+      </c>
+      <c r="G6">
+        <v>-161.49</v>
+      </c>
+      <c r="H6">
+        <v>-168.34</v>
+      </c>
+      <c r="I6">
+        <v>-197.48</v>
+      </c>
+      <c r="J6">
+        <v>-181.21</v>
+      </c>
+      <c r="K6">
+        <v>-189.51</v>
+      </c>
+      <c r="L6">
+        <v>-198.57</v>
+      </c>
+      <c r="M6">
+        <v>-232.45</v>
+      </c>
+      <c r="N6">
+        <v>-264.07</v>
+      </c>
+      <c r="O6">
+        <v>-1275.67</v>
+      </c>
+      <c r="P6">
+        <v>-1584.52</v>
+      </c>
+      <c r="Q6">
+        <v>-1709.57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>-142.44999999999999</v>
+      </c>
+      <c r="C7">
+        <v>-142.58000000000001</v>
+      </c>
+      <c r="D7">
+        <v>-135.44</v>
+      </c>
+      <c r="E7">
+        <v>-146.65</v>
+      </c>
+      <c r="F7">
+        <v>-169.26</v>
+      </c>
+      <c r="G7">
+        <v>-194.92</v>
+      </c>
+      <c r="H7">
+        <v>-206.67</v>
+      </c>
+      <c r="I7">
+        <v>-171.46</v>
+      </c>
+      <c r="J7">
+        <v>-190.58</v>
+      </c>
+      <c r="K7">
+        <v>-189.5</v>
+      </c>
+      <c r="L7">
+        <v>-197.18</v>
+      </c>
+      <c r="M7">
+        <v>-222.47</v>
+      </c>
+      <c r="N7">
+        <v>-266.5</v>
+      </c>
+      <c r="O7">
+        <v>-340.74</v>
+      </c>
+      <c r="P7">
+        <v>-1512.64</v>
+      </c>
+      <c r="Q7">
+        <v>-1629.09</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>-140.85</v>
+      </c>
+      <c r="C8">
+        <v>-136.06</v>
+      </c>
+      <c r="D8">
+        <v>-166.29</v>
+      </c>
+      <c r="E8">
+        <v>-154.53</v>
+      </c>
+      <c r="F8">
+        <v>-173.56</v>
+      </c>
+      <c r="G8">
+        <v>-185.65</v>
+      </c>
+      <c r="H8">
+        <v>-168.65</v>
+      </c>
+      <c r="I8">
+        <v>-192</v>
+      </c>
+      <c r="J8">
+        <v>-176.62</v>
+      </c>
+      <c r="K8">
+        <v>-197.22</v>
+      </c>
+      <c r="L8">
+        <v>-204.54</v>
+      </c>
+      <c r="M8">
+        <v>-207.54</v>
+      </c>
+      <c r="N8">
+        <v>-240.16</v>
+      </c>
+      <c r="O8">
+        <v>-293</v>
+      </c>
+      <c r="P8">
+        <v>-1516.29</v>
+      </c>
+      <c r="Q8">
+        <v>-1648.88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>-113.12</v>
+      </c>
+      <c r="C9">
+        <v>-101</v>
+      </c>
+      <c r="D9">
+        <v>-105.06</v>
+      </c>
+      <c r="E9">
+        <v>-142.74</v>
+      </c>
+      <c r="F9">
+        <v>-162.66</v>
+      </c>
+      <c r="G9">
+        <v>-157.93</v>
+      </c>
+      <c r="H9">
+        <v>-142.01</v>
+      </c>
+      <c r="I9">
+        <v>-164.66</v>
+      </c>
+      <c r="J9">
+        <v>-190.16</v>
+      </c>
+      <c r="K9">
+        <v>-189.32</v>
+      </c>
+      <c r="L9">
+        <v>-202.37</v>
+      </c>
+      <c r="M9">
+        <v>-194.2</v>
+      </c>
+      <c r="N9">
+        <v>-762.94</v>
+      </c>
+      <c r="O9">
+        <v>-1452.16</v>
+      </c>
+      <c r="P9">
+        <v>-1610.83</v>
+      </c>
+      <c r="Q9">
+        <v>-1698.27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>-180.46</v>
+      </c>
       <c r="C10">
-        <v>2</v>
+        <v>-152.76</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>-177.3</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>-163.54</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>-169</v>
       </c>
       <c r="G10">
-        <v>6</v>
+        <v>-203.31</v>
       </c>
       <c r="H10">
-        <v>7</v>
+        <v>-179.57</v>
       </c>
       <c r="I10">
-        <v>8</v>
+        <v>-192.61</v>
       </c>
       <c r="J10">
-        <v>9.81</v>
+        <v>-205.91</v>
       </c>
       <c r="K10">
-        <v>11</v>
+        <v>-239.01</v>
       </c>
       <c r="L10">
-        <v>12</v>
+        <v>-204.37</v>
       </c>
       <c r="M10">
-        <v>13</v>
+        <v>-225.95</v>
       </c>
       <c r="N10">
-        <v>14</v>
+        <v>-222.7</v>
       </c>
       <c r="O10">
-        <v>15</v>
+        <v>-325.89</v>
       </c>
       <c r="P10">
-        <v>16</v>
+        <v>-1404.22</v>
       </c>
       <c r="Q10">
-        <v>17</v>
+        <v>-1582.08</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>-148.11000000000001</v>
+      </c>
+      <c r="C11">
+        <v>-106.46</v>
+      </c>
+      <c r="D11">
+        <v>-134.36000000000001</v>
+      </c>
+      <c r="E11">
+        <v>-128.4</v>
+      </c>
+      <c r="F11">
+        <v>-159.53</v>
+      </c>
+      <c r="G11">
+        <v>-197.43</v>
+      </c>
+      <c r="H11">
+        <v>-157.37</v>
+      </c>
+      <c r="I11">
+        <v>-175.41</v>
+      </c>
+      <c r="J11">
+        <v>-193.79</v>
+      </c>
+      <c r="K11">
+        <v>-198.9</v>
+      </c>
+      <c r="L11">
+        <v>-196.09</v>
+      </c>
+      <c r="M11">
+        <v>-200.45</v>
+      </c>
+      <c r="N11">
+        <v>-237.91</v>
+      </c>
+      <c r="O11">
+        <v>-421.96</v>
+      </c>
+      <c r="P11">
+        <v>-1516.6</v>
+      </c>
+      <c r="Q11">
+        <v>-1772.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <v>7</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <v>9.81</v>
+      </c>
+      <c r="K13">
+        <v>11</v>
+      </c>
+      <c r="L13">
+        <v>12</v>
+      </c>
+      <c r="M13">
+        <v>13</v>
+      </c>
+      <c r="N13">
+        <v>14</v>
+      </c>
+      <c r="O13">
+        <v>15</v>
+      </c>
+      <c r="P13">
+        <v>16</v>
+      </c>
+      <c r="Q13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <f>AVERAGE(B2:B9)</f>
-        <v>-194.38749999999999</v>
-      </c>
-      <c r="C11">
-        <f t="shared" ref="C11:P11" si="0">AVERAGE(C2:C9)</f>
-        <v>-191.83875</v>
-      </c>
-      <c r="D11">
+      <c r="B14">
+        <f>AVERAGE(B2:B11)</f>
+        <v>-134.446</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:Q14" si="0">AVERAGE(C2:C11)</f>
+        <v>-126.43200000000002</v>
+      </c>
+      <c r="D14">
         <f t="shared" si="0"/>
-        <v>-182.14875000000001</v>
-      </c>
-      <c r="E11">
+        <v>-137.16399999999999</v>
+      </c>
+      <c r="E14">
         <f t="shared" si="0"/>
-        <v>-180.8725</v>
-      </c>
-      <c r="F11">
+        <v>-143.74699999999999</v>
+      </c>
+      <c r="F14">
         <f t="shared" si="0"/>
-        <v>-189.86875000000001</v>
-      </c>
-      <c r="G11">
+        <v>-162.54400000000001</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="0"/>
-        <v>-196.5675</v>
-      </c>
-      <c r="H11">
+        <v>-176.85300000000001</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="0"/>
-        <v>-211.73750000000001</v>
-      </c>
-      <c r="I11">
+        <v>-170.24900000000002</v>
+      </c>
+      <c r="I14">
         <f t="shared" si="0"/>
-        <v>-195.185</v>
-      </c>
-      <c r="J11">
+        <v>-186.14800000000002</v>
+      </c>
+      <c r="J14">
         <f t="shared" si="0"/>
-        <v>-215.47250000000003</v>
-      </c>
-      <c r="K11">
+        <v>-194.95500000000001</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="0"/>
-        <v>-216.58875</v>
-      </c>
-      <c r="L11">
+        <v>-205.99299999999999</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="0"/>
-        <v>-228.09875</v>
-      </c>
-      <c r="M11">
+        <v>-221.80700000000002</v>
+      </c>
+      <c r="M14">
         <f t="shared" si="0"/>
-        <v>-256.51375000000002</v>
-      </c>
-      <c r="N11">
+        <v>-228.94399999999996</v>
+      </c>
+      <c r="N14">
         <f t="shared" si="0"/>
-        <v>-944.80124999999998</v>
-      </c>
-      <c r="O11">
+        <v>-316.56899999999996</v>
+      </c>
+      <c r="O14">
         <f t="shared" si="0"/>
-        <v>-1483.8687499999996</v>
-      </c>
-      <c r="P11">
+        <v>-784.322</v>
+      </c>
+      <c r="P14">
         <f t="shared" si="0"/>
-        <v>-1644.6925000000001</v>
-      </c>
-      <c r="Q11">
-        <f>AVERAGE(Q2:Q9)</f>
-        <v>-1790.8275000000003</v>
+        <v>-1543.931</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>-1681.5169999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Write changes to from raw to grav
</commit_message>
<xml_diff>
--- a/pendulum/random_full_grav/random_full_grav.xlsx
+++ b/pendulum/random_full_grav/random_full_grav.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/random_full_grav/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6264A7-145A-5B4A-8F8C-73AD94ACEE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78BAFAB-1691-E148-93B3-57B8A8C8FA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="13" sheetId="2" r:id="rId2"/>
-    <sheet name="15" sheetId="3" r:id="rId3"/>
+    <sheet name="13 (old)" sheetId="1" r:id="rId1"/>
+    <sheet name="15" sheetId="2" r:id="rId2"/>
+    <sheet name="13" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
-  <si>
-    <t>empty</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Ind</t>
   </si>
@@ -98,6 +95,45 @@
   </si>
   <si>
     <t>conditional(add(add(y, y), add(y, x)), add(add(add(y, x), add(add(x, y), add(x, x))), add(add(y, add(vel, x)), conditional(conditional(x, add(conditional(add(conditional(add(add(x, conditional(add(x, x), add(add(vel, x), conditional(y, vel)))), add(conditional(conditional(vel, add(add(y, x), conditional(x, vel))), add(conditional(conditional(vel, y), vel), conditional(x, vel))), vel)), vel), add(conditional(vel, y), add(vel, x))), conditional(conditional(conditional(conditional(x, add(conditional(y, x), add(y, vel))), conditional(add(x, x), conditional(y, y))), add(conditional(add(vel, vel), x), conditional(x, vel))), y)), add(conditional(conditional(x, y), conditional(x, y)), conditional(conditional(x, add(conditional(vel, conditional(conditional(conditional(x, x), add(add(vel, y), add(add(add(y, y), add(vel, x)), add(y, vel)))), add(x, y))), add(conditional(add(conditional(conditional(y, add(vel, x)), conditional(x, y)), add(add(vel, add(add(x, y), add(y, vel))), conditional(add(x, y), x))), conditional(add(vel, y), x)), conditional(add(x, vel), add(vel, x))))), add(conditional(add(y, vel), conditional(conditional(vel, conditional(conditional(vel, conditional(conditional(x, vel), vel)), add(conditional(conditional(add(y, x), x), y), conditional(x, x)))), add(conditional(y, y), conditional(y, x)))), add(x, y)))))), add(conditional(add(y, vel), conditional(conditional(vel, conditional(add(y, add(y, add(vel, x))), add(conditional(add(add(conditional(x, y), add(x, vel)), add(conditional(conditional(vel, conditional(conditional(vel, x), add(vel, vel))), add(conditional(add(x, vel), vel), conditional(x, vel))), vel)), vel), add(conditional(vel, x), add(conditional(x, y), x))))), y)), conditional(conditional(x, conditional(conditional(x, vel), y)), add(add(x, y), conditional(y, conditional(x, x)))))))))</t>
+  </si>
+  <si>
+    <t>conditional(add(y, add(conditional(y, y), add(x, y))), add(add(vel, add(vel, add(add(add(conditional(add(vel, add(add(add(conditional(add(x, x), x), add(add(x, y), x)), x), add(x, conditional(vel, y)))), x), add(add(x, y), add(x, x))), x), y))), add(x, add(x, x))))</t>
+  </si>
+  <si>
+    <t>conditional(add(y, y), add(vel, add(y, add(add(add(y, x), add(x, x)), vel))))</t>
+  </si>
+  <si>
+    <t>conditional(add(add(y, conditional(x, vel)), y), add(y, add(add(x, add(vel, x)), add(add(conditional(x, x), add(conditional(x, conditional(conditional(x, x), conditional(x, vel))), add(x, y))), x))))</t>
+  </si>
+  <si>
+    <t>conditional(add(y, add(y, y)), add(add(add(add(add(add(x, add(x, add(add(add(x, add(conditional(x, add(y, vel)), add(conditional(x, x), x))), add(x, conditional(x, conditional(y, y)))), vel))), add(x, add(add(x, add(y, x)), y))), vel), x), add(x, add(x, conditional(y, conditional(vel, vel))))), vel))</t>
+  </si>
+  <si>
+    <t>conditional(add(y, y), add(conditional(y, conditional(conditional(y, y), add(conditional(y, conditional(y, x)), add(vel, x)))), add(x, add(add(add(add(x, y), conditional(x, x)), x), add(vel, x)))))</t>
+  </si>
+  <si>
+    <t>conditional(add(y, y), add(add(add(y, add(conditional(conditional(x, add(x, x)), conditional(add(x, x), conditional(conditional(y, vel), x))), vel)), add(add(x, conditional(x, x)), add(y, x))), x))</t>
+  </si>
+  <si>
+    <t>conditional(add(add(y, y), y), add(add(add(add(x, y), vel), x), add(add(add(add(y, vel), x), add(add(conditional(conditional(x, conditional(conditional(y, conditional(add(vel, x), conditional(y, vel))), vel)), add(conditional(add(y, vel), vel), y)), add(conditional(y, y), conditional(conditional(x, x), x))), x)), add(x, add(x, x)))))</t>
+  </si>
+  <si>
+    <t>conditional(add(y, y), add(add(add(x, y), add(add(add(conditional(conditional(x, y), add(add(y, vel), x)), add(conditional(add(x, vel), conditional(vel, x)), x)), vel), add(add(x, x), y))), add(x, vel)))</t>
+  </si>
+  <si>
+    <t>conditional(add(y, y), add(add(conditional(conditional(vel, vel), add(add(conditional(conditional(conditional(vel, vel), conditional(y, vel)), conditional(vel, conditional(add(y, vel), add(add(x, vel), add(conditional(y, x), y))))), add(add(add(vel, x), add(x, y)), x)), add(y, add(x, add(x, vel))))), add(add(add(vel, x), add(x, y)), x)), add(y, add(x, vel))))</t>
+  </si>
+  <si>
+    <t>add(conditional(add(y, add(y, y)), add(add(x, add(add(add(x, x), add(conditional(conditional(y, conditional(add(x, x), add(x, x))), conditional(conditional(conditional(x, y), conditional(vel, vel)), vel)), x)), add(add(add(conditional(add(conditional(y, vel), conditional(vel, y)), x), add(x, vel)), y), vel))), vel)), conditional(conditional(conditional(x, conditional(vel, x)), y), add(x, x)))</t>
+  </si>
+  <si>
+    <t>conditional(add(y, add(y, y)), add(add(add(x, y), add(conditional(conditional(x, add(add(y, x), add(y, add(conditional(add(conditional(add(vel, conditional(x, y)), conditional(y, x)), y), conditional(x, y)), add(add(x, y), add(conditional(conditional(x, x), add(x, x)), conditional(conditional(x, y), add(conditional(vel, add(y, x)), conditional(y, vel))))))))), conditional(add(add(conditional(conditional(x, y), add(y, x)), add(add(conditional(add(vel, vel), add(vel, x)), conditional(add(y, y), add(x, x))), add(add(x, vel), add(add(add(vel, conditional(conditional(vel, vel), x)), add(vel, y)), conditional(conditional(y, vel), add(vel, x)))))), add(conditional(x, vel), vel)), add(conditional(conditional(y, x), add(y, x)), add(add(add(y, x), vel), add(add(y, add(x, add(conditional(conditional(vel, vel), add(x, x)), add(x, add(x, add(add(conditional(vel, y), x), conditional(x, x))))))), add(add(conditional(conditional(x, x), add(add(x, vel), x)), conditional(add(vel, x), conditional(y, add(x, conditional(y, vel))))), add(x, y))))))), add(add(x, y), add(x, add(x, vel))))), y))</t>
+  </si>
+  <si>
+    <t>conditional(add(y, add(conditional(x, x), add(y, y))), add(add(x, add(conditional(conditional(add(add(x, y), x), y), conditional(y, y)), add(add(x, x), add(y, vel)))), add(add(conditional(conditional(conditional(conditional(vel, x), y), add(y, vel)), conditional(x, y)), add(add(add(x, x), conditional(conditional(y, vel), conditional(conditional(y, y), add(y, y)))), add(add(add(x, y), add(vel, vel)), x))), x)))</t>
+  </si>
+  <si>
+    <t>conditional(add(conditional(y, conditional(conditional(y, x), add(conditional(y, add(add(add(add(add(vel, vel), x), add(x, vel)), add(vel, x)), conditional(add(conditional(conditional(y, add(vel, y)), add(conditional(y, add(y, x)), conditional(vel, x))), conditional(x, conditional(vel, y))), conditional(vel, conditional(y, vel))))), conditional(vel, add(add(x, y), conditional(x, vel)))))), add(y, y)), add(add(add(add(y, x), add(vel, add(x, x))), y), conditional(add(conditional(y, conditional(conditional(y, x), add(conditional(y, add(add(add(conditional(vel, y), add(vel, vel)), x), x)), y))), conditional(x, x)), x)))</t>
   </si>
 </sst>
 </file>
@@ -197,6 +233,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15'!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -211,7 +258,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'13'!$B$11:$Q$11</c:f>
+              <c:f>'15'!$B$13:$Q$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -268,86 +315,65 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'9.81'!#REF!</c:f>
+              <c:f>'15'!$B$14:$Q$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>-194.38749999999999</c:v>
+                  <c:v>-134.446</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-191.83875</c:v>
+                  <c:v>-126.43200000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-182.14875000000001</c:v>
+                  <c:v>-137.16399999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-180.8725</c:v>
+                  <c:v>-143.74699999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-189.86875000000001</c:v>
+                  <c:v>-162.54400000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-196.5675</c:v>
+                  <c:v>-176.85300000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-211.73750000000001</c:v>
+                  <c:v>-170.24900000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-195.185</c:v>
+                  <c:v>-186.14800000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-215.4725</c:v>
+                  <c:v>-194.95500000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-216.58875</c:v>
+                  <c:v>-205.99299999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-228.09875</c:v>
+                  <c:v>-221.80700000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-256.51375000000002</c:v>
+                  <c:v>-228.94399999999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-944.80124999999998</c:v>
+                  <c:v>-316.56899999999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-1483.8687500000001</c:v>
+                  <c:v>-784.322</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1644.6925000000001</c:v>
+                  <c:v>-1543.931</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1790.8275000000001</c:v>
+                  <c:v>-1681.5169999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredSeriesTitle>
-                <c15:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>'9.81'!#REF!</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>Fit</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c15:tx>
-              </c15:filteredSeriesTitle>
-            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1887-E741-82C3-8E172A801702}"/>
+              <c16:uniqueId val="{00000000-F6F5-2048-8A04-5D1C2133FEDF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -360,11 +386,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1074713648"/>
-        <c:axId val="1531991088"/>
+        <c:axId val="1208166048"/>
+        <c:axId val="1208154272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1074713648"/>
+        <c:axId val="1208166048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -407,7 +433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1531991088"/>
+        <c:crossAx val="1208154272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -415,9 +441,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1531991088"/>
+        <c:axId val="1208154272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="-2000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -466,7 +493,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1074713648"/>
+        <c:crossAx val="1208166048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -553,7 +580,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'15'!$A$14</c:f>
+              <c:f>'13'!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -576,7 +603,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'15'!$B$13:$Q$13</c:f>
+              <c:f>'13'!$B$16:$Q$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -633,57 +660,57 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'15'!$B$14:$Q$14</c:f>
+              <c:f>'13'!$B$17:$Q$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>-134.446</c:v>
+                  <c:v>-161.05000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-126.43200000000002</c:v>
+                  <c:v>-144.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-137.16399999999999</c:v>
+                  <c:v>-154.85</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-143.74699999999999</c:v>
+                  <c:v>-151.53</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-162.54400000000001</c:v>
+                  <c:v>-168.55</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-176.85300000000001</c:v>
+                  <c:v>-186.86</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-170.24900000000002</c:v>
+                  <c:v>-184.81</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-186.14800000000002</c:v>
+                  <c:v>-201.46</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-194.95500000000001</c:v>
+                  <c:v>-219.42</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-205.99299999999999</c:v>
+                  <c:v>-215.04</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-221.80700000000002</c:v>
+                  <c:v>-219.11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-228.94399999999996</c:v>
+                  <c:v>-246.13</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-316.56899999999996</c:v>
+                  <c:v>-1016.62</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-784.322</c:v>
+                  <c:v>-1482.42</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1543.931</c:v>
+                  <c:v>-1666.6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1681.5169999999998</c:v>
+                  <c:v>-1801.21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -691,7 +718,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7878-9D48-AC6F-BF602411C75A}"/>
+              <c16:uniqueId val="{00000000-95E8-D342-8ED1-85D2D3E38404}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -704,16 +731,30 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1208166048"/>
-        <c:axId val="1208154272"/>
+        <c:axId val="1342768928"/>
+        <c:axId val="1342846688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1208166048"/>
+        <c:axId val="1342768928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -751,7 +792,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1208154272"/>
+        <c:crossAx val="1342846688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -759,10 +800,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1208154272"/>
+        <c:axId val="1342846688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="-2000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -811,9 +851,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1208166048"/>
+        <c:crossAx val="1342768928"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1427,16 +1467,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1468,23 +1508,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>450850</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>15532</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>20818</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:colOff>359226</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>145737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D636F47-F0BE-B307-8B17-8D3E18D5A6C9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B7CE4D0-09A8-77EB-51E4-0A00CCAA27FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1500,6 +1540,402 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>592667</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>338667</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>198967</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C667DEE8-79C3-D589-ED48-00F782C740E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="592667" y="3945467"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>643467</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101599</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>389467</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>12699</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55980403-C1DC-4D19-4791-87E686937B6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6739467" y="3962399"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>67734</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>491067</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>198967</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ECEFEE6-B8A5-D35A-DC3E-FE91AEC6003B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12937067" y="3945467"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>291475</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>104098</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>137409</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>113467</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{338866BB-9E75-07B8-3FAB-AFB822B7D913}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18945901" y="4059836"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>458033</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>145738</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>303967</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>155107</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE21FE5A-1136-BA42-DACE-11567800D09E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="458033" y="8890000"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>624589</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>166557</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>470524</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>175926</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8E192FD-3E54-9EB4-C8B9-47890E9F67FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6620655" y="8910819"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>145738</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>145738</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>657902</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>155107</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31DA19E3-1278-015D-6F94-D43E88B6EF9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12804099" y="8890000"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>312295</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>62460</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>158229</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>71829</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B221D54-6065-7EB5-A1E5-6366F49D89D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18966721" y="8806722"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>374754</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>62458</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>220688</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>71827</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{559FDC0A-816B-28F2-3C16-FDFA50B9B196}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="374754" y="13803442"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1802,21 +2238,612 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="93" workbookViewId="0">
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9.81</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>12</v>
+      </c>
+      <c r="M1">
+        <v>13</v>
+      </c>
+      <c r="N1">
+        <v>14</v>
+      </c>
+      <c r="O1">
+        <v>15</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="Q1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-144.79</v>
+      </c>
+      <c r="C2">
+        <v>-165.52</v>
+      </c>
+      <c r="D2">
+        <v>-141.1</v>
+      </c>
+      <c r="E2">
+        <v>-177.26</v>
+      </c>
+      <c r="F2">
+        <v>-158.30000000000001</v>
+      </c>
+      <c r="G2">
+        <v>-171.49</v>
+      </c>
+      <c r="H2">
+        <v>-187.61</v>
+      </c>
+      <c r="I2">
+        <v>-183.55</v>
+      </c>
+      <c r="J2">
+        <v>-202.67</v>
+      </c>
+      <c r="K2">
+        <v>-244.01</v>
+      </c>
+      <c r="L2">
+        <v>-217.68</v>
+      </c>
+      <c r="M2">
+        <v>-232.62</v>
+      </c>
+      <c r="N2">
+        <v>-729.37</v>
+      </c>
+      <c r="O2">
+        <v>-1419.86</v>
+      </c>
+      <c r="P2">
+        <v>-1648.98</v>
+      </c>
+      <c r="Q2">
+        <v>-1749.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>-174.77</v>
+      </c>
+      <c r="C3">
+        <v>-145.4</v>
+      </c>
+      <c r="D3">
+        <v>-182.09</v>
+      </c>
+      <c r="E3">
+        <v>-125.31</v>
+      </c>
+      <c r="F3">
+        <v>-148.87</v>
+      </c>
+      <c r="G3">
+        <v>-165.02</v>
+      </c>
+      <c r="H3">
+        <v>-160.97</v>
+      </c>
+      <c r="I3">
+        <v>-167.19</v>
+      </c>
+      <c r="J3">
+        <v>-206.26</v>
+      </c>
+      <c r="K3">
+        <v>-185.81</v>
+      </c>
+      <c r="L3">
+        <v>-213.59</v>
+      </c>
+      <c r="M3">
+        <v>-239.81</v>
+      </c>
+      <c r="N3">
+        <v>-1115.77</v>
+      </c>
+      <c r="O3">
+        <v>-1481.79</v>
+      </c>
+      <c r="P3">
+        <v>-1594.41</v>
+      </c>
+      <c r="Q3">
+        <v>-1762.18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-138.22</v>
+      </c>
+      <c r="C4">
+        <v>-130.41999999999999</v>
+      </c>
+      <c r="D4">
+        <v>-173.22</v>
+      </c>
+      <c r="E4">
+        <v>-170.63</v>
+      </c>
+      <c r="F4">
+        <v>-177.82</v>
+      </c>
+      <c r="G4">
+        <v>-184.06</v>
+      </c>
+      <c r="H4">
+        <v>-197.36</v>
+      </c>
+      <c r="I4">
+        <v>-193.96</v>
+      </c>
+      <c r="J4">
+        <v>-212.77</v>
+      </c>
+      <c r="K4">
+        <v>-255.75</v>
+      </c>
+      <c r="L4">
+        <v>-294.14</v>
+      </c>
+      <c r="M4">
+        <v>-324.68</v>
+      </c>
+      <c r="N4">
+        <v>-1391.5</v>
+      </c>
+      <c r="O4">
+        <v>-1616.33</v>
+      </c>
+      <c r="P4">
+        <v>-1683.17</v>
+      </c>
+      <c r="Q4">
+        <v>-1856.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-211.15</v>
+      </c>
+      <c r="C5">
+        <v>-228.47</v>
+      </c>
+      <c r="D5">
+        <v>-235.07</v>
+      </c>
+      <c r="E5">
+        <v>-206.46</v>
+      </c>
+      <c r="F5">
+        <v>-255.92</v>
+      </c>
+      <c r="G5">
+        <v>-216.91</v>
+      </c>
+      <c r="H5">
+        <v>-261.95999999999998</v>
+      </c>
+      <c r="I5">
+        <v>-213.46</v>
+      </c>
+      <c r="J5">
+        <v>-195.3</v>
+      </c>
+      <c r="K5">
+        <v>-181.47</v>
+      </c>
+      <c r="L5">
+        <v>-186.06</v>
+      </c>
+      <c r="M5">
+        <v>-209.38</v>
+      </c>
+      <c r="N5">
+        <v>-258.75</v>
+      </c>
+      <c r="O5">
+        <v>-1340.06</v>
+      </c>
+      <c r="P5">
+        <v>-1636.01</v>
+      </c>
+      <c r="Q5">
+        <v>-1804.48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-187.85</v>
+      </c>
+      <c r="C6">
+        <v>-173.05</v>
+      </c>
+      <c r="D6">
+        <v>-154.04</v>
+      </c>
+      <c r="E6">
+        <v>-161.04</v>
+      </c>
+      <c r="F6">
+        <v>-174.16</v>
+      </c>
+      <c r="G6">
+        <v>-177.7</v>
+      </c>
+      <c r="H6">
+        <v>-195.09</v>
+      </c>
+      <c r="I6">
+        <v>-220.15</v>
+      </c>
+      <c r="J6">
+        <v>-251</v>
+      </c>
+      <c r="K6">
+        <v>-240.41</v>
+      </c>
+      <c r="L6">
+        <v>-253.25</v>
+      </c>
+      <c r="M6">
+        <v>-307.17</v>
+      </c>
+      <c r="N6">
+        <v>-1341.49</v>
+      </c>
+      <c r="O6">
+        <v>-1632.21</v>
+      </c>
+      <c r="P6">
+        <v>-1739.47</v>
+      </c>
+      <c r="Q6">
+        <v>-1840.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-297.8</v>
+      </c>
+      <c r="C7">
+        <v>-316.06</v>
+      </c>
+      <c r="D7">
+        <v>-236.99</v>
+      </c>
+      <c r="E7">
+        <v>-203.92</v>
+      </c>
+      <c r="F7">
+        <v>-161.91</v>
+      </c>
+      <c r="G7">
+        <v>-177.67</v>
+      </c>
+      <c r="H7">
+        <v>-172.71</v>
+      </c>
+      <c r="I7">
+        <v>-166.92</v>
+      </c>
+      <c r="J7">
+        <v>-190.67</v>
+      </c>
+      <c r="K7">
+        <v>-184.74</v>
+      </c>
+      <c r="L7">
+        <v>-205.05</v>
+      </c>
+      <c r="M7">
+        <v>-226.69</v>
+      </c>
+      <c r="N7">
+        <v>-300.07</v>
+      </c>
+      <c r="O7">
+        <v>-1394.58</v>
+      </c>
+      <c r="P7">
+        <v>-1476.16</v>
+      </c>
+      <c r="Q7">
+        <v>-1743.69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-182.13</v>
+      </c>
+      <c r="C8">
+        <v>-197.23</v>
+      </c>
+      <c r="D8">
+        <v>-171.95</v>
+      </c>
+      <c r="E8">
+        <v>-213.96</v>
+      </c>
+      <c r="F8">
+        <v>-274.73</v>
+      </c>
+      <c r="G8">
+        <v>-281.07</v>
+      </c>
+      <c r="H8">
+        <v>-274.41000000000003</v>
+      </c>
+      <c r="I8">
+        <v>-227.74</v>
+      </c>
+      <c r="J8">
+        <v>-236.7</v>
+      </c>
+      <c r="K8">
+        <v>-207.46</v>
+      </c>
+      <c r="L8">
+        <v>-239.05</v>
+      </c>
+      <c r="M8">
+        <v>-281.19</v>
+      </c>
+      <c r="N8">
+        <v>-1390.66</v>
+      </c>
+      <c r="O8">
+        <v>-1508.14</v>
+      </c>
+      <c r="P8">
+        <v>-1695.53</v>
+      </c>
+      <c r="Q8">
+        <v>-1765.78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>-218.39</v>
+      </c>
+      <c r="C9">
+        <v>-178.56</v>
+      </c>
+      <c r="D9">
+        <v>-162.72999999999999</v>
+      </c>
+      <c r="E9">
+        <v>-188.4</v>
+      </c>
+      <c r="F9">
+        <v>-167.24</v>
+      </c>
+      <c r="G9">
+        <v>-198.62</v>
+      </c>
+      <c r="H9">
+        <v>-243.79</v>
+      </c>
+      <c r="I9">
+        <v>-188.51</v>
+      </c>
+      <c r="J9">
+        <v>-228.41</v>
+      </c>
+      <c r="K9">
+        <v>-233.06</v>
+      </c>
+      <c r="L9">
+        <v>-215.97</v>
+      </c>
+      <c r="M9">
+        <v>-230.57</v>
+      </c>
+      <c r="N9">
+        <v>-1030.8</v>
+      </c>
+      <c r="O9">
+        <v>-1477.98</v>
+      </c>
+      <c r="P9">
+        <v>-1683.81</v>
+      </c>
+      <c r="Q9">
+        <v>-1803.85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <v>7</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <v>9.81</v>
+      </c>
+      <c r="K13">
+        <v>11</v>
+      </c>
+      <c r="L13">
+        <v>12</v>
+      </c>
+      <c r="M13">
+        <v>13</v>
+      </c>
+      <c r="N13">
+        <v>14</v>
+      </c>
+      <c r="O13">
+        <v>15</v>
+      </c>
+      <c r="P13">
+        <v>16</v>
+      </c>
+      <c r="Q13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:Q14" si="0">AVERAGE(B2:B11)</f>
+        <v>-194.38749999999999</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>-191.83875</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-182.14875000000001</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>-180.8725</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>-189.86875000000001</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>-196.5675</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>-211.73750000000001</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>-195.185</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>-215.47250000000003</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>-216.58875</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>-228.09875</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>-256.51375000000002</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>-944.80124999999998</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>-1483.8687499999996</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>-1644.6925000000001</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>-1790.8275000000003</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1824,15 +2851,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -1885,529 +2912,532 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>-155.97</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>-123.65</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>-173.25</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>-144.44999999999999</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>-156.19</v>
       </c>
       <c r="G2">
-        <v>6</v>
+        <v>-178.47</v>
       </c>
       <c r="H2">
-        <v>7</v>
+        <v>-187.63</v>
       </c>
       <c r="I2">
-        <v>8</v>
+        <v>-168.83</v>
       </c>
       <c r="J2">
-        <v>9.81</v>
+        <v>-177</v>
       </c>
       <c r="K2">
-        <v>11</v>
+        <v>-196.58</v>
       </c>
       <c r="L2">
-        <v>12</v>
+        <v>-199.08</v>
       </c>
       <c r="M2">
-        <v>13</v>
+        <v>-236.5</v>
       </c>
       <c r="N2">
-        <v>14</v>
+        <v>-258.51</v>
       </c>
       <c r="O2">
-        <v>15</v>
+        <v>-1092.1199999999999</v>
       </c>
       <c r="P2">
-        <v>16</v>
+        <v>-1600.51</v>
       </c>
       <c r="Q2">
-        <v>17</v>
+        <v>-1712.94</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <v>-144.79</v>
+        <v>-85.38</v>
       </c>
       <c r="C3">
-        <v>-165.52</v>
+        <v>-95.44</v>
       </c>
       <c r="D3">
-        <v>-141.1</v>
+        <v>-95.54</v>
       </c>
       <c r="E3">
-        <v>-177.26</v>
+        <v>-107.69</v>
       </c>
       <c r="F3">
-        <v>-158.30000000000001</v>
+        <v>-114.55</v>
       </c>
       <c r="G3">
-        <v>-171.49</v>
+        <v>-138.68</v>
       </c>
       <c r="H3">
-        <v>-187.61</v>
+        <v>-145.88</v>
       </c>
       <c r="I3">
-        <v>-183.55</v>
+        <v>-176.41</v>
       </c>
       <c r="J3">
-        <v>-202.67</v>
+        <v>-223.04</v>
       </c>
       <c r="K3">
-        <v>-244.01</v>
+        <v>-268.73</v>
       </c>
       <c r="L3">
-        <v>-217.68</v>
+        <v>-391.07</v>
       </c>
       <c r="M3">
-        <v>-232.62</v>
+        <v>-344.78</v>
       </c>
       <c r="N3">
-        <v>-729.37</v>
+        <v>-416.86</v>
       </c>
       <c r="O3">
-        <v>-1419.86</v>
+        <v>-575.91</v>
       </c>
       <c r="P3">
-        <v>-1648.98</v>
+        <v>-1556.9</v>
       </c>
       <c r="Q3">
-        <v>-1749.75</v>
+        <v>-1727.9</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B4">
-        <v>-174.77</v>
+        <v>-134.38</v>
       </c>
       <c r="C4">
-        <v>-145.4</v>
+        <v>-153.08000000000001</v>
       </c>
       <c r="D4">
-        <v>-182.09</v>
+        <v>-126.96</v>
       </c>
       <c r="E4">
-        <v>-125.31</v>
+        <v>-154.02000000000001</v>
       </c>
       <c r="F4">
-        <v>-148.87</v>
+        <v>-191.94</v>
       </c>
       <c r="G4">
-        <v>-165.02</v>
+        <v>-182.74</v>
       </c>
       <c r="H4">
-        <v>-160.97</v>
+        <v>-181.74</v>
       </c>
       <c r="I4">
-        <v>-167.19</v>
+        <v>-220.15</v>
       </c>
       <c r="J4">
-        <v>-206.26</v>
+        <v>-195.63</v>
       </c>
       <c r="K4">
-        <v>-185.81</v>
+        <v>-197.6</v>
       </c>
       <c r="L4">
-        <v>-213.59</v>
+        <v>-230.94</v>
       </c>
       <c r="M4">
-        <v>-239.81</v>
+        <v>-215.05</v>
       </c>
       <c r="N4">
-        <v>-1115.77</v>
+        <v>-241.29</v>
       </c>
       <c r="O4">
-        <v>-1481.79</v>
+        <v>-1264.43</v>
       </c>
       <c r="P4">
-        <v>-1594.41</v>
+        <v>-1565.99</v>
       </c>
       <c r="Q4">
-        <v>-1762.18</v>
+        <v>-1686.79</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B5">
-        <v>-138.22</v>
+        <v>-126.81</v>
       </c>
       <c r="C5">
-        <v>-130.41999999999999</v>
+        <v>-121.9</v>
       </c>
       <c r="D5">
-        <v>-173.22</v>
+        <v>-132.53</v>
       </c>
       <c r="E5">
-        <v>-170.63</v>
+        <v>-133.19999999999999</v>
       </c>
       <c r="F5">
-        <v>-177.82</v>
+        <v>-152.81</v>
       </c>
       <c r="G5">
-        <v>-184.06</v>
+        <v>-167.91</v>
       </c>
       <c r="H5">
-        <v>-197.36</v>
+        <v>-164.63</v>
       </c>
       <c r="I5">
-        <v>-193.96</v>
+        <v>-202.47</v>
       </c>
       <c r="J5">
-        <v>-212.77</v>
+        <v>-215.61</v>
       </c>
       <c r="K5">
-        <v>-255.75</v>
+        <v>-193.56</v>
       </c>
       <c r="L5">
-        <v>-294.14</v>
+        <v>-193.86</v>
       </c>
       <c r="M5">
-        <v>-324.68</v>
+        <v>-210.05</v>
       </c>
       <c r="N5">
-        <v>-1391.5</v>
+        <v>-254.75</v>
       </c>
       <c r="O5">
-        <v>-1616.33</v>
+        <v>-801.34</v>
       </c>
       <c r="P5">
-        <v>-1683.17</v>
+        <v>-1570.81</v>
       </c>
       <c r="Q5">
-        <v>-1856.04</v>
+        <v>-1647.61</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B6">
-        <v>-211.15</v>
+        <v>-116.93</v>
       </c>
       <c r="C6">
-        <v>-228.47</v>
+        <v>-131.38999999999999</v>
       </c>
       <c r="D6">
-        <v>-235.07</v>
+        <v>-124.91</v>
       </c>
       <c r="E6">
-        <v>-206.46</v>
+        <v>-162.25</v>
       </c>
       <c r="F6">
-        <v>-255.92</v>
+        <v>-175.94</v>
       </c>
       <c r="G6">
-        <v>-216.91</v>
+        <v>-161.49</v>
       </c>
       <c r="H6">
-        <v>-261.95999999999998</v>
+        <v>-168.34</v>
       </c>
       <c r="I6">
-        <v>-213.46</v>
+        <v>-197.48</v>
       </c>
       <c r="J6">
-        <v>-195.3</v>
+        <v>-181.21</v>
       </c>
       <c r="K6">
-        <v>-181.47</v>
+        <v>-189.51</v>
       </c>
       <c r="L6">
-        <v>-186.06</v>
+        <v>-198.57</v>
       </c>
       <c r="M6">
-        <v>-209.38</v>
+        <v>-232.45</v>
       </c>
       <c r="N6">
-        <v>-258.75</v>
+        <v>-264.07</v>
       </c>
       <c r="O6">
-        <v>-1340.06</v>
+        <v>-1275.67</v>
       </c>
       <c r="P6">
-        <v>-1636.01</v>
+        <v>-1584.52</v>
       </c>
       <c r="Q6">
-        <v>-1804.48</v>
+        <v>-1709.57</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <v>-187.85</v>
+        <v>-142.44999999999999</v>
       </c>
       <c r="C7">
-        <v>-173.05</v>
+        <v>-142.58000000000001</v>
       </c>
       <c r="D7">
-        <v>-154.04</v>
+        <v>-135.44</v>
       </c>
       <c r="E7">
-        <v>-161.04</v>
+        <v>-146.65</v>
       </c>
       <c r="F7">
-        <v>-174.16</v>
+        <v>-169.26</v>
       </c>
       <c r="G7">
-        <v>-177.7</v>
+        <v>-194.92</v>
       </c>
       <c r="H7">
-        <v>-195.09</v>
+        <v>-206.67</v>
       </c>
       <c r="I7">
-        <v>-220.15</v>
+        <v>-171.46</v>
       </c>
       <c r="J7">
-        <v>-251</v>
+        <v>-190.58</v>
       </c>
       <c r="K7">
-        <v>-240.41</v>
+        <v>-189.5</v>
       </c>
       <c r="L7">
-        <v>-253.25</v>
+        <v>-197.18</v>
       </c>
       <c r="M7">
-        <v>-307.17</v>
+        <v>-222.47</v>
       </c>
       <c r="N7">
-        <v>-1341.49</v>
+        <v>-266.5</v>
       </c>
       <c r="O7">
-        <v>-1632.21</v>
+        <v>-340.74</v>
       </c>
       <c r="P7">
-        <v>-1739.47</v>
+        <v>-1512.64</v>
       </c>
       <c r="Q7">
-        <v>-1840.85</v>
+        <v>-1629.09</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B8">
-        <v>-297.8</v>
+        <v>-140.85</v>
       </c>
       <c r="C8">
-        <v>-316.06</v>
+        <v>-136.06</v>
       </c>
       <c r="D8">
-        <v>-236.99</v>
+        <v>-166.29</v>
       </c>
       <c r="E8">
-        <v>-203.92</v>
+        <v>-154.53</v>
       </c>
       <c r="F8">
-        <v>-161.91</v>
+        <v>-173.56</v>
       </c>
       <c r="G8">
-        <v>-177.67</v>
+        <v>-185.65</v>
       </c>
       <c r="H8">
-        <v>-172.71</v>
+        <v>-168.65</v>
       </c>
       <c r="I8">
-        <v>-166.92</v>
+        <v>-192</v>
       </c>
       <c r="J8">
-        <v>-190.67</v>
+        <v>-176.62</v>
       </c>
       <c r="K8">
-        <v>-184.74</v>
+        <v>-197.22</v>
       </c>
       <c r="L8">
-        <v>-205.05</v>
+        <v>-204.54</v>
       </c>
       <c r="M8">
-        <v>-226.69</v>
+        <v>-207.54</v>
       </c>
       <c r="N8">
-        <v>-300.07</v>
+        <v>-240.16</v>
       </c>
       <c r="O8">
-        <v>-1394.58</v>
+        <v>-293</v>
       </c>
       <c r="P8">
-        <v>-1476.16</v>
+        <v>-1516.29</v>
       </c>
       <c r="Q8">
-        <v>-1743.69</v>
+        <v>-1648.88</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>-182.13</v>
+        <v>-113.12</v>
       </c>
       <c r="C9">
-        <v>-197.23</v>
+        <v>-101</v>
       </c>
       <c r="D9">
-        <v>-171.95</v>
+        <v>-105.06</v>
       </c>
       <c r="E9">
-        <v>-213.96</v>
+        <v>-142.74</v>
       </c>
       <c r="F9">
-        <v>-274.73</v>
+        <v>-162.66</v>
       </c>
       <c r="G9">
-        <v>-281.07</v>
+        <v>-157.93</v>
       </c>
       <c r="H9">
-        <v>-274.41000000000003</v>
+        <v>-142.01</v>
       </c>
       <c r="I9">
-        <v>-227.74</v>
+        <v>-164.66</v>
       </c>
       <c r="J9">
-        <v>-236.7</v>
+        <v>-190.16</v>
       </c>
       <c r="K9">
-        <v>-207.46</v>
+        <v>-189.32</v>
       </c>
       <c r="L9">
-        <v>-239.05</v>
+        <v>-202.37</v>
       </c>
       <c r="M9">
-        <v>-281.19</v>
+        <v>-194.2</v>
       </c>
       <c r="N9">
-        <v>-1390.66</v>
+        <v>-762.94</v>
       </c>
       <c r="O9">
-        <v>-1508.14</v>
+        <v>-1452.16</v>
       </c>
       <c r="P9">
-        <v>-1695.53</v>
+        <v>-1610.83</v>
       </c>
       <c r="Q9">
-        <v>-1765.78</v>
+        <v>-1698.27</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B10">
-        <v>-218.39</v>
+        <v>-180.46</v>
       </c>
       <c r="C10">
-        <v>-178.56</v>
+        <v>-152.76</v>
       </c>
       <c r="D10">
-        <v>-162.72999999999999</v>
+        <v>-177.3</v>
       </c>
       <c r="E10">
-        <v>-188.4</v>
+        <v>-163.54</v>
       </c>
       <c r="F10">
-        <v>-167.24</v>
+        <v>-169</v>
       </c>
       <c r="G10">
-        <v>-198.62</v>
+        <v>-203.31</v>
       </c>
       <c r="H10">
-        <v>-243.79</v>
+        <v>-179.57</v>
       </c>
       <c r="I10">
-        <v>-188.51</v>
+        <v>-192.61</v>
       </c>
       <c r="J10">
-        <v>-228.41</v>
+        <v>-205.91</v>
       </c>
       <c r="K10">
-        <v>-233.06</v>
+        <v>-239.01</v>
       </c>
       <c r="L10">
-        <v>-215.97</v>
+        <v>-204.37</v>
       </c>
       <c r="M10">
-        <v>-230.57</v>
+        <v>-225.95</v>
       </c>
       <c r="N10">
-        <v>-1030.8</v>
+        <v>-222.7</v>
       </c>
       <c r="O10">
-        <v>-1477.98</v>
+        <v>-325.89</v>
       </c>
       <c r="P10">
-        <v>-1683.81</v>
+        <v>-1404.22</v>
       </c>
       <c r="Q10">
-        <v>-1803.85</v>
+        <v>-1582.08</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
       <c r="B11">
-        <v>1</v>
+        <v>-148.11000000000001</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>-106.46</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>-134.36000000000001</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>-128.4</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>-159.53</v>
       </c>
       <c r="G11">
-        <v>6</v>
+        <v>-197.43</v>
       </c>
       <c r="H11">
-        <v>7</v>
+        <v>-157.37</v>
       </c>
       <c r="I11">
-        <v>8</v>
+        <v>-175.41</v>
       </c>
       <c r="J11">
-        <v>9.81</v>
+        <v>-193.79</v>
       </c>
       <c r="K11">
-        <v>11</v>
+        <v>-198.9</v>
       </c>
       <c r="L11">
-        <v>12</v>
+        <v>-196.09</v>
       </c>
       <c r="M11">
-        <v>13</v>
+        <v>-200.45</v>
       </c>
       <c r="N11">
-        <v>14</v>
+        <v>-237.91</v>
       </c>
       <c r="O11">
-        <v>15</v>
+        <v>-421.96</v>
       </c>
       <c r="P11">
-        <v>16</v>
+        <v>-1516.6</v>
       </c>
       <c r="Q11">
-        <v>17</v>
+        <v>-1772.04</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -2462,71 +3492,71 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14">
-        <f>AVERAGE(B2:B11)</f>
-        <v>-155.31</v>
+        <f t="shared" ref="B14:Q14" si="0">AVERAGE(B2:B11)</f>
+        <v>-134.446</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:Q14" si="0">AVERAGE(C2:C11)</f>
-        <v>-153.071</v>
+        <f t="shared" si="0"/>
+        <v>-126.43200000000002</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-145.119</v>
+        <v>-137.16399999999999</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>-143.898</v>
+        <v>-143.74699999999999</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>-150.89500000000001</v>
+        <v>-162.54400000000001</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>-156.054</v>
+        <v>-176.85300000000001</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>-167.99</v>
+        <v>-170.24900000000002</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>-154.548</v>
+        <v>-186.14800000000002</v>
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>-170.41600000000003</v>
+        <v>-194.95500000000001</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>-171.071</v>
+        <v>-205.99299999999999</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
-        <v>-180.07900000000001</v>
+        <v>-221.80700000000002</v>
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>-202.61100000000002</v>
+        <v>-228.94399999999996</v>
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
-        <v>-753.04099999999994</v>
+        <v>-316.56899999999996</v>
       </c>
       <c r="O14">
         <f t="shared" si="0"/>
-        <v>-1184.0949999999998</v>
+        <v>-784.322</v>
       </c>
       <c r="P14">
         <f t="shared" si="0"/>
-        <v>-1312.5540000000001</v>
+        <v>-1543.931</v>
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
-        <v>-1429.2620000000002</v>
+        <v>-1681.5169999999998</v>
       </c>
     </row>
   </sheetData>
@@ -2537,17 +3567,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
+      <selection activeCell="X73" sqref="X73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -2600,651 +3630,810 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B2">
-        <v>-155.97</v>
+        <v>-439.56</v>
       </c>
       <c r="C2">
-        <v>-123.65</v>
+        <v>-386.96</v>
       </c>
       <c r="D2">
-        <v>-173.25</v>
+        <v>-395.09</v>
       </c>
       <c r="E2">
-        <v>-144.44999999999999</v>
+        <v>-459.18</v>
       </c>
       <c r="F2">
-        <v>-156.19</v>
+        <v>-388.2</v>
       </c>
       <c r="G2">
-        <v>-178.47</v>
+        <v>-334.02</v>
       </c>
       <c r="H2">
-        <v>-187.63</v>
+        <v>-290.52</v>
       </c>
       <c r="I2">
-        <v>-168.83</v>
+        <v>-280.41000000000003</v>
       </c>
       <c r="J2">
-        <v>-177</v>
+        <v>-226.23</v>
       </c>
       <c r="K2">
-        <v>-196.58</v>
+        <v>-239.31</v>
       </c>
       <c r="L2">
-        <v>-199.08</v>
+        <v>-245.25</v>
       </c>
       <c r="M2">
-        <v>-236.5</v>
+        <v>-334.11</v>
       </c>
       <c r="N2">
-        <v>-258.51</v>
+        <v>-339.51</v>
       </c>
       <c r="O2">
-        <v>-1092.1199999999999</v>
+        <v>-938.81</v>
       </c>
       <c r="P2">
-        <v>-1600.51</v>
+        <v>-1645.14</v>
       </c>
       <c r="Q2">
-        <v>-1712.94</v>
+        <v>-1771.41</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>-85.38</v>
+        <v>-161.44</v>
       </c>
       <c r="C3">
-        <v>-95.44</v>
+        <v>-144.6</v>
       </c>
       <c r="D3">
-        <v>-95.54</v>
+        <v>-154.85</v>
       </c>
       <c r="E3">
-        <v>-107.69</v>
+        <v>-173.85</v>
       </c>
       <c r="F3">
-        <v>-114.55</v>
+        <v>-168.55</v>
       </c>
       <c r="G3">
-        <v>-138.68</v>
+        <v>-206.05</v>
       </c>
       <c r="H3">
-        <v>-145.88</v>
+        <v>-219.13</v>
       </c>
       <c r="I3">
-        <v>-176.41</v>
+        <v>-220.42</v>
       </c>
       <c r="J3">
-        <v>-223.04</v>
+        <v>-265.66000000000003</v>
       </c>
       <c r="K3">
-        <v>-268.73</v>
+        <v>-259.12</v>
       </c>
       <c r="L3">
-        <v>-391.07</v>
+        <v>-1130.6400000000001</v>
       </c>
       <c r="M3">
-        <v>-344.78</v>
+        <v>-1360.67</v>
       </c>
       <c r="N3">
-        <v>-416.86</v>
+        <v>-1549.48</v>
       </c>
       <c r="O3">
-        <v>-575.91</v>
+        <v>-1694.02</v>
       </c>
       <c r="P3">
-        <v>-1556.9</v>
+        <v>-1793.85</v>
       </c>
       <c r="Q3">
-        <v>-1727.9</v>
+        <v>-1886.73</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B4">
-        <v>-134.38</v>
+        <v>-196.41</v>
       </c>
       <c r="C4">
-        <v>-153.08000000000001</v>
+        <v>-129.99</v>
       </c>
       <c r="D4">
-        <v>-126.96</v>
+        <v>-116.02</v>
       </c>
       <c r="E4">
-        <v>-154.02000000000001</v>
+        <v>-143.91999999999999</v>
       </c>
       <c r="F4">
-        <v>-191.94</v>
+        <v>-149.65</v>
       </c>
       <c r="G4">
-        <v>-182.74</v>
+        <v>-159.72999999999999</v>
       </c>
       <c r="H4">
-        <v>-181.74</v>
+        <v>-184.81</v>
       </c>
       <c r="I4">
-        <v>-220.15</v>
+        <v>-170.35</v>
       </c>
       <c r="J4">
-        <v>-195.63</v>
+        <v>-180.54</v>
       </c>
       <c r="K4">
-        <v>-197.6</v>
+        <v>-203.52</v>
       </c>
       <c r="L4">
-        <v>-230.94</v>
+        <v>-210.48</v>
       </c>
       <c r="M4">
-        <v>-215.05</v>
+        <v>-233.34</v>
       </c>
       <c r="N4">
-        <v>-241.29</v>
+        <v>-1285.3699999999999</v>
       </c>
       <c r="O4">
-        <v>-1264.43</v>
+        <v>-1563.02</v>
       </c>
       <c r="P4">
-        <v>-1565.99</v>
+        <v>-1736.02</v>
       </c>
       <c r="Q4">
-        <v>-1686.79</v>
+        <v>-1879.7</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B5">
-        <v>-126.81</v>
+        <v>-161.05000000000001</v>
       </c>
       <c r="C5">
-        <v>-121.9</v>
+        <v>-145.08000000000001</v>
       </c>
       <c r="D5">
-        <v>-132.53</v>
+        <v>-154.12</v>
       </c>
       <c r="E5">
-        <v>-133.19999999999999</v>
+        <v>-145.31</v>
       </c>
       <c r="F5">
-        <v>-152.81</v>
+        <v>-166.2</v>
       </c>
       <c r="G5">
-        <v>-167.91</v>
+        <v>-186.8</v>
       </c>
       <c r="H5">
-        <v>-164.63</v>
+        <v>-181.35</v>
       </c>
       <c r="I5">
-        <v>-202.47</v>
+        <v>-172.42</v>
       </c>
       <c r="J5">
-        <v>-215.61</v>
+        <v>-189.76</v>
       </c>
       <c r="K5">
-        <v>-193.56</v>
+        <v>-181.48</v>
       </c>
       <c r="L5">
-        <v>-193.86</v>
+        <v>-193.52</v>
       </c>
       <c r="M5">
-        <v>-210.05</v>
+        <v>-216.19</v>
       </c>
       <c r="N5">
-        <v>-254.75</v>
+        <v>-349.99</v>
       </c>
       <c r="O5">
-        <v>-801.34</v>
+        <v>-1351.79</v>
       </c>
       <c r="P5">
-        <v>-1570.81</v>
+        <v>-1543.63</v>
       </c>
       <c r="Q5">
-        <v>-1647.61</v>
+        <v>-1710.69</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B6">
-        <v>-116.93</v>
+        <v>-244.2</v>
       </c>
       <c r="C6">
-        <v>-131.38999999999999</v>
+        <v>-159.78</v>
       </c>
       <c r="D6">
-        <v>-124.91</v>
+        <v>-159.43</v>
       </c>
       <c r="E6">
-        <v>-162.25</v>
+        <v>-166.34</v>
       </c>
       <c r="F6">
-        <v>-175.94</v>
+        <v>-178.58</v>
       </c>
       <c r="G6">
-        <v>-161.49</v>
+        <v>-187.3</v>
       </c>
       <c r="H6">
-        <v>-168.34</v>
+        <v>-188.49</v>
       </c>
       <c r="I6">
-        <v>-197.48</v>
+        <v>-218.03</v>
       </c>
       <c r="J6">
-        <v>-181.21</v>
+        <v>-238.22</v>
       </c>
       <c r="K6">
-        <v>-189.51</v>
+        <v>-215.04</v>
       </c>
       <c r="L6">
-        <v>-198.57</v>
+        <v>-224.66</v>
       </c>
       <c r="M6">
-        <v>-232.45</v>
+        <v>-240.94</v>
       </c>
       <c r="N6">
-        <v>-264.07</v>
+        <v>-1016.62</v>
       </c>
       <c r="O6">
-        <v>-1275.67</v>
+        <v>-1498.51</v>
       </c>
       <c r="P6">
-        <v>-1584.52</v>
+        <v>-1606.45</v>
       </c>
       <c r="Q6">
-        <v>-1709.57</v>
+        <v>-1870.03</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B7">
-        <v>-142.44999999999999</v>
+        <v>-179.03</v>
       </c>
       <c r="C7">
-        <v>-142.58000000000001</v>
+        <v>-166.78</v>
       </c>
       <c r="D7">
-        <v>-135.44</v>
+        <v>-175.45</v>
       </c>
       <c r="E7">
-        <v>-146.65</v>
+        <v>-151.53</v>
       </c>
       <c r="F7">
-        <v>-169.26</v>
+        <v>-166.5</v>
       </c>
       <c r="G7">
-        <v>-194.92</v>
+        <v>-198.34</v>
       </c>
       <c r="H7">
-        <v>-206.67</v>
+        <v>-223.61</v>
       </c>
       <c r="I7">
-        <v>-171.46</v>
+        <v>-220.82</v>
       </c>
       <c r="J7">
-        <v>-190.58</v>
+        <v>-216.27</v>
       </c>
       <c r="K7">
-        <v>-189.5</v>
+        <v>-232.06</v>
       </c>
       <c r="L7">
-        <v>-197.18</v>
+        <v>-222.81</v>
       </c>
       <c r="M7">
-        <v>-222.47</v>
+        <v>-289.17</v>
       </c>
       <c r="N7">
-        <v>-266.5</v>
+        <v>-1162.96</v>
       </c>
       <c r="O7">
-        <v>-340.74</v>
+        <v>-1571</v>
       </c>
       <c r="P7">
-        <v>-1512.64</v>
+        <v>-1682.03</v>
       </c>
       <c r="Q7">
-        <v>-1629.09</v>
+        <v>-1834.89</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B8">
-        <v>-140.85</v>
+        <v>-136.05000000000001</v>
       </c>
       <c r="C8">
-        <v>-136.06</v>
+        <v>-126.06</v>
       </c>
       <c r="D8">
-        <v>-166.29</v>
+        <v>-151.41</v>
       </c>
       <c r="E8">
-        <v>-154.53</v>
+        <v>-147.19999999999999</v>
       </c>
       <c r="F8">
-        <v>-173.56</v>
+        <v>-154.56</v>
       </c>
       <c r="G8">
-        <v>-185.65</v>
+        <v>-166.96</v>
       </c>
       <c r="H8">
-        <v>-168.65</v>
+        <v>-182.92</v>
       </c>
       <c r="I8">
-        <v>-192</v>
+        <v>-179.43</v>
       </c>
       <c r="J8">
-        <v>-176.62</v>
+        <v>-177.99</v>
       </c>
       <c r="K8">
-        <v>-197.22</v>
+        <v>-194.98</v>
       </c>
       <c r="L8">
-        <v>-204.54</v>
+        <v>-188.43</v>
       </c>
       <c r="M8">
-        <v>-207.54</v>
+        <v>-206.22</v>
       </c>
       <c r="N8">
-        <v>-240.16</v>
+        <v>-281.55</v>
       </c>
       <c r="O8">
-        <v>-293</v>
+        <v>-1336.49</v>
       </c>
       <c r="P8">
-        <v>-1516.29</v>
+        <v>-1576.13</v>
       </c>
       <c r="Q8">
-        <v>-1648.88</v>
+        <v>-1746.56</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B9">
-        <v>-113.12</v>
+        <v>-182.64</v>
       </c>
       <c r="C9">
-        <v>-101</v>
+        <v>-177.37</v>
       </c>
       <c r="D9">
-        <v>-105.06</v>
+        <v>-161.41999999999999</v>
       </c>
       <c r="E9">
-        <v>-142.74</v>
+        <v>-163.53</v>
       </c>
       <c r="F9">
-        <v>-162.66</v>
+        <v>-177.96</v>
       </c>
       <c r="G9">
-        <v>-157.93</v>
+        <v>-187.78</v>
       </c>
       <c r="H9">
-        <v>-142.01</v>
+        <v>-196.36</v>
       </c>
       <c r="I9">
-        <v>-164.66</v>
+        <v>-205.07</v>
       </c>
       <c r="J9">
-        <v>-190.16</v>
+        <v>-219.42</v>
       </c>
       <c r="K9">
-        <v>-189.32</v>
+        <v>-218.05</v>
       </c>
       <c r="L9">
-        <v>-202.37</v>
+        <v>-205.8</v>
       </c>
       <c r="M9">
-        <v>-194.2</v>
+        <v>-234.93</v>
       </c>
       <c r="N9">
-        <v>-762.94</v>
+        <v>-1104.8900000000001</v>
       </c>
       <c r="O9">
-        <v>-1452.16</v>
+        <v>-1470.47</v>
       </c>
       <c r="P9">
-        <v>-1610.83</v>
+        <v>-1673.23</v>
       </c>
       <c r="Q9">
-        <v>-1698.27</v>
+        <v>-1805.12</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B10">
-        <v>-180.46</v>
+        <v>-137.54</v>
       </c>
       <c r="C10">
-        <v>-152.76</v>
+        <v>-167.58</v>
       </c>
       <c r="D10">
-        <v>-177.3</v>
+        <v>-167.04</v>
       </c>
       <c r="E10">
-        <v>-163.54</v>
+        <v>-164.37</v>
       </c>
       <c r="F10">
-        <v>-169</v>
+        <v>-156.25</v>
       </c>
       <c r="G10">
-        <v>-203.31</v>
+        <v>-198.92</v>
       </c>
       <c r="H10">
-        <v>-179.57</v>
+        <v>-179.28</v>
       </c>
       <c r="I10">
-        <v>-192.61</v>
+        <v>-205.48</v>
       </c>
       <c r="J10">
-        <v>-205.91</v>
+        <v>-222.5</v>
       </c>
       <c r="K10">
-        <v>-239.01</v>
+        <v>-209.62</v>
       </c>
       <c r="L10">
-        <v>-204.37</v>
+        <v>-224.38</v>
       </c>
       <c r="M10">
-        <v>-225.95</v>
+        <v>-324.05</v>
       </c>
       <c r="N10">
-        <v>-222.7</v>
+        <v>-1331.22</v>
       </c>
       <c r="O10">
-        <v>-325.89</v>
+        <v>-1594.65</v>
       </c>
       <c r="P10">
-        <v>-1404.22</v>
+        <v>-1740.42</v>
       </c>
       <c r="Q10">
-        <v>-1582.08</v>
+        <v>-1801.21</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B11">
-        <v>-148.11000000000001</v>
+        <v>-128.66</v>
       </c>
       <c r="C11">
-        <v>-106.46</v>
+        <v>-128.82</v>
       </c>
       <c r="D11">
-        <v>-134.36000000000001</v>
+        <v>-146.76</v>
       </c>
       <c r="E11">
-        <v>-128.4</v>
+        <v>-137.41</v>
       </c>
       <c r="F11">
-        <v>-159.53</v>
+        <v>-207.06</v>
       </c>
       <c r="G11">
-        <v>-197.43</v>
+        <v>-186.86</v>
       </c>
       <c r="H11">
-        <v>-157.37</v>
+        <v>-187.11</v>
       </c>
       <c r="I11">
-        <v>-175.41</v>
+        <v>-201.46</v>
       </c>
       <c r="J11">
-        <v>-193.79</v>
+        <v>-237.12</v>
       </c>
       <c r="K11">
-        <v>-198.9</v>
+        <v>-293.99</v>
       </c>
       <c r="L11">
-        <v>-196.09</v>
+        <v>-271.33999999999997</v>
       </c>
       <c r="M11">
-        <v>-200.45</v>
+        <v>-344.28</v>
       </c>
       <c r="N11">
-        <v>-237.91</v>
+        <v>-1222.94</v>
       </c>
       <c r="O11">
-        <v>-421.96</v>
+        <v>-1459.7</v>
       </c>
       <c r="P11">
-        <v>-1516.6</v>
+        <v>-1560.77</v>
       </c>
       <c r="Q11">
-        <v>-1772.04</v>
+        <v>-1647.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>-145.19</v>
+      </c>
+      <c r="C12">
+        <v>-117.25</v>
+      </c>
+      <c r="D12">
+        <v>-148.66</v>
+      </c>
+      <c r="E12">
+        <v>-130.78</v>
+      </c>
+      <c r="F12">
+        <v>-177.13</v>
+      </c>
+      <c r="G12">
+        <v>-186.79</v>
+      </c>
+      <c r="H12">
+        <v>-173.05</v>
+      </c>
+      <c r="I12">
+        <v>-189.67</v>
+      </c>
+      <c r="J12">
+        <v>-168.19</v>
+      </c>
+      <c r="K12">
+        <v>-182.31</v>
+      </c>
+      <c r="L12">
+        <v>-198.04</v>
+      </c>
+      <c r="M12">
+        <v>-224.09</v>
+      </c>
+      <c r="N12">
+        <v>-255.22</v>
+      </c>
+      <c r="O12">
+        <v>-1302.1600000000001</v>
+      </c>
+      <c r="P12">
+        <v>-1490.29</v>
+      </c>
+      <c r="Q12">
+        <v>-1684.83</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
       <c r="B13">
-        <v>1</v>
+        <v>-142.19999999999999</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>-138.30000000000001</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>-155.22999999999999</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>-159.5</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>-187.26</v>
       </c>
       <c r="G13">
-        <v>6</v>
+        <v>-182.83</v>
       </c>
       <c r="H13">
-        <v>7</v>
+        <v>-181.06</v>
       </c>
       <c r="I13">
-        <v>8</v>
+        <v>-194.99</v>
       </c>
       <c r="J13">
-        <v>9.81</v>
+        <v>-221.73</v>
       </c>
       <c r="K13">
-        <v>11</v>
+        <v>-227.1</v>
       </c>
       <c r="L13">
-        <v>12</v>
+        <v>-219.11</v>
       </c>
       <c r="M13">
-        <v>13</v>
+        <v>-261.7</v>
       </c>
       <c r="N13">
-        <v>14</v>
+        <v>-814.94</v>
       </c>
       <c r="O13">
-        <v>15</v>
+        <v>-1536.52</v>
       </c>
       <c r="P13">
-        <v>16</v>
+        <v>-1720.53</v>
       </c>
       <c r="Q13">
-        <v>17</v>
+        <v>-1859.14</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B14">
-        <f>AVERAGE(B2:B11)</f>
-        <v>-134.446</v>
+        <v>-113.56</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:Q14" si="0">AVERAGE(C2:C11)</f>
-        <v>-126.43200000000002</v>
+        <v>-118.71</v>
       </c>
       <c r="D14">
+        <v>-109.63</v>
+      </c>
+      <c r="E14">
+        <v>-127.46</v>
+      </c>
+      <c r="F14">
+        <v>-133.97</v>
+      </c>
+      <c r="G14">
+        <v>-139.16</v>
+      </c>
+      <c r="H14">
+        <v>-153.18</v>
+      </c>
+      <c r="I14">
+        <v>-167.51</v>
+      </c>
+      <c r="J14">
+        <v>-188.74</v>
+      </c>
+      <c r="K14">
+        <v>-187.25</v>
+      </c>
+      <c r="L14">
+        <v>-211.39</v>
+      </c>
+      <c r="M14">
+        <v>-246.13</v>
+      </c>
+      <c r="N14">
+        <v>-935.17</v>
+      </c>
+      <c r="O14">
+        <v>-1482.42</v>
+      </c>
+      <c r="P14">
+        <v>-1666.6</v>
+      </c>
+      <c r="Q14">
+        <v>-1714.91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>6</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
+      </c>
+      <c r="I16">
+        <v>8</v>
+      </c>
+      <c r="J16">
+        <v>9.81</v>
+      </c>
+      <c r="K16">
+        <v>11</v>
+      </c>
+      <c r="L16">
+        <v>12</v>
+      </c>
+      <c r="M16">
+        <v>13</v>
+      </c>
+      <c r="N16">
+        <v>14</v>
+      </c>
+      <c r="O16">
+        <v>15</v>
+      </c>
+      <c r="P16">
+        <v>16</v>
+      </c>
+      <c r="Q16">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <f>MEDIAN(B2:B14)</f>
+        <v>-161.05000000000001</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:Q17" si="0">MEDIAN(C2:C14)</f>
+        <v>-144.6</v>
+      </c>
+      <c r="D17">
         <f t="shared" si="0"/>
-        <v>-137.16399999999999</v>
-      </c>
-      <c r="E14">
+        <v>-154.85</v>
+      </c>
+      <c r="E17">
         <f t="shared" si="0"/>
-        <v>-143.74699999999999</v>
-      </c>
-      <c r="F14">
+        <v>-151.53</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="0"/>
-        <v>-162.54400000000001</v>
-      </c>
-      <c r="G14">
+        <v>-168.55</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="0"/>
-        <v>-176.85300000000001</v>
-      </c>
-      <c r="H14">
+        <v>-186.86</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="0"/>
-        <v>-170.24900000000002</v>
-      </c>
-      <c r="I14">
+        <v>-184.81</v>
+      </c>
+      <c r="I17">
         <f t="shared" si="0"/>
-        <v>-186.14800000000002</v>
-      </c>
-      <c r="J14">
+        <v>-201.46</v>
+      </c>
+      <c r="J17">
         <f t="shared" si="0"/>
-        <v>-194.95500000000001</v>
-      </c>
-      <c r="K14">
+        <v>-219.42</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="0"/>
-        <v>-205.99299999999999</v>
-      </c>
-      <c r="L14">
+        <v>-215.04</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="0"/>
-        <v>-221.80700000000002</v>
-      </c>
-      <c r="M14">
+        <v>-219.11</v>
+      </c>
+      <c r="M17">
         <f t="shared" si="0"/>
-        <v>-228.94399999999996</v>
-      </c>
-      <c r="N14">
+        <v>-246.13</v>
+      </c>
+      <c r="N17">
         <f t="shared" si="0"/>
-        <v>-316.56899999999996</v>
-      </c>
-      <c r="O14">
+        <v>-1016.62</v>
+      </c>
+      <c r="O17">
         <f t="shared" si="0"/>
-        <v>-784.322</v>
-      </c>
-      <c r="P14">
+        <v>-1482.42</v>
+      </c>
+      <c r="P17">
         <f t="shared" si="0"/>
-        <v>-1543.931</v>
-      </c>
-      <c r="Q14">
+        <v>-1666.6</v>
+      </c>
+      <c r="Q17">
         <f t="shared" si="0"/>
-        <v>-1681.5169999999998</v>
+        <v>-1801.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>